<commit_message>
GKv3 (EtoForms): Improving of compatibility
</commit_message>
<xml_diff>
--- a/dev_info/gk_compatibility_matrix.xlsx
+++ b/dev_info/gk_compatibility_matrix.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKS\shared\gkdev\-devel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C1EA0D-D7AB-459D-BA48-B5BEB26E17FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Compatibility Matrix" sheetId="2" r:id="rId1"/>
@@ -18,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Compatibility Matrix'!$A$2:$H$96</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,71 +28,198 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={0C8C2A0A-09FB-4B08-999F-C16384413ED6}</author>
     <author>tc={03199625-ADA0-4544-BEED-2EC70A7B7558}</author>
     <author>tc={B204A590-8F59-45C2-AF46-0C451D79A7F2}</author>
+    <author>tc={FC38DB41-2593-4AE3-890A-83FAE8D7361F}</author>
     <author>tc={CABCC935-D353-49C6-BF7B-26945C3B7EEC}</author>
+    <author>tc={4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}</author>
     <author>tc={2E4E5FAA-8920-4E1C-B04E-22732D846631}</author>
+    <author>tc={08B0E8B2-B025-4593-86AB-65151186337D}</author>
     <author>tc={D1AD9B46-69A2-4F80-ADD4-0B51A5891E85}</author>
     <author>tc={BD118A23-46B1-45EB-A479-612E3372B34F}</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{0C8C2A0A-09FB-4B08-999F-C16384413ED6}">
+    <comment ref="D6" authorId="0">
       <text>
-        <t>[Цепочка примечаний]
-Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
-Комментарий:
-    coordinates from ScrollPanel, unify</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>coordinates from ScrollPanel, unify</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{03199625-ADA0-4544-BEED-2EC70A7B7558}">
+    <comment ref="D7" authorId="1">
       <text>
-        <t>[Цепочка примечаний]
-Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
-Комментарий:
-    no metafiles</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>no metafiles</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="2" shapeId="0" xr:uid="{B204A590-8F59-45C2-AF46-0C451D79A7F2}">
+    <comment ref="D10" authorId="2">
       <text>
-        <t>[Цепочка примечаний]
-Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
-Комментарий:
-    many small inaccuracies</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>many small inaccuracies</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="3" shapeId="0" xr:uid="{CABCC935-D353-49C6-BF7B-26945C3B7EEC}">
+    <comment ref="D14" authorId="3">
       <text>
-        <t>[Цепочка примечаний]
-Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
-Комментарий:
-    no dragdrop</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>many small inaccuracies</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D51" authorId="4" shapeId="0" xr:uid="{2E4E5FAA-8920-4E1C-B04E-22732D846631}">
+    <comment ref="D20" authorId="4">
       <text>
-        <t>[Цепочка примечаний]
-Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
-Комментарий:
-    first image not fitted to window</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>no dragdrop</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D66" authorId="5" shapeId="0" xr:uid="{D1AD9B46-69A2-4F80-ADD4-0B51A5891E85}">
+    <comment ref="D32" authorId="5">
       <text>
-        <t>[Цепочка примечаний]
-Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
-Комментарий:
-    not works lists</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>require toolbar's combobox and dropdownbtn</t>
+        </r>
       </text>
     </comment>
-    <comment ref="D68" authorId="6" shapeId="0" xr:uid="{BD118A23-46B1-45EB-A479-612E3372B34F}">
+    <comment ref="D38" authorId="6">
       <text>
-        <t>[Цепочка примечаний]
-Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
-Комментарий:
-    lines without arrow's caps</t>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>dialog scale inaccuracy</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D51" authorId="6">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>first image not fitted to window</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D54" authorId="7">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>no charts</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D66" authorId="8">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>not works lists</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D68" authorId="9">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>lines without arrow's caps</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D77" authorId="8">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>not works slidepanel</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -106,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="117">
   <si>
     <t>Module</t>
   </si>
@@ -126,9 +247,6 @@
     <t>GKProgram.cs</t>
   </si>
   <si>
-    <t>GKUI\WFAppHost.cs</t>
-  </si>
-  <si>
     <t>GKUI\Components\ACOptionsControl.cs</t>
   </si>
   <si>
@@ -375,18 +493,6 @@
     <t>GKUI\Components\UIHelper.cs</t>
   </si>
   <si>
-    <t>GKUI\Components\WFGfxProvider.cs</t>
-  </si>
-  <si>
-    <t>GKUI\Components\WFGfxRenderer.cs</t>
-  </si>
-  <si>
-    <t>GKUI\Components\WFStdDialogs.cs</t>
-  </si>
-  <si>
-    <t>GKUI\Components\WinUITimer.cs</t>
-  </si>
-  <si>
     <t>GKUI\Components\WizardPages.cs</t>
   </si>
   <si>
@@ -412,21 +518,6 @@
   </si>
   <si>
     <t>GKUI\Components\ObservableExtList.cs</t>
-  </si>
-  <si>
-    <t>GKUI\Components\EtoStdDialogs.cs</t>
-  </si>
-  <si>
-    <t>GKUI\Components\EUITimer.cs</t>
-  </si>
-  <si>
-    <t>GKUI\Components\EtoGraphics.cs</t>
-  </si>
-  <si>
-    <t>GKUI\Components\EtoGfxProvider.cs</t>
-  </si>
-  <si>
-    <t>GKUI\Components\EtoGfxRenderer.cs</t>
   </si>
   <si>
     <t>GKUI\Components\GKMenuItem.cs</t>
@@ -491,19 +582,52 @@
     <t>Functions&amp;Design</t>
   </si>
   <si>
-    <t>EtoAppHost.cs</t>
-  </si>
-  <si>
     <t>Implemented</t>
   </si>
   <si>
     <t>Verified</t>
+  </si>
+  <si>
+    <t>partial</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\WinUITimer.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\WFStdDialogs.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\EUITimer.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\EtoStdDialogs.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\EtoGraphics.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\EtoGfxRenderer.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\EtoGfxProvider.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\WFGfxProvider.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\WFGfxRenderer.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\WFAppHost.cs</t>
+  </si>
+  <si>
+    <t>GKUI\Platform\EtoAppHost.cs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -1110,24 +1234,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -1462,7 +1586,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1479,11 +1603,20 @@
   <threadedComment ref="D10" dT="2021-05-08T22:17:18.54" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{B204A590-8F59-45C2-AF46-0C451D79A7F2}">
     <text>many small inaccuracies</text>
   </threadedComment>
+  <threadedComment ref="D14" dT="2021-05-08T22:17:18.54" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{FC38DB41-2593-4AE3-890A-83FAE8D7361F}">
+    <text>many small inaccuracies</text>
+  </threadedComment>
   <threadedComment ref="D20" dT="2021-05-07T20:37:27.60" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{CABCC935-D353-49C6-BF7B-26945C3B7EEC}">
     <text>no dragdrop</text>
   </threadedComment>
+  <threadedComment ref="D32" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}">
+    <text>require toolbar's combobox and dropdownbtn</text>
+  </threadedComment>
   <threadedComment ref="D51" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{2E4E5FAA-8920-4E1C-B04E-22732D846631}">
     <text>first image not fitted to window</text>
+  </threadedComment>
+  <threadedComment ref="D54" dT="2021-05-08T19:23:42.84" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{08B0E8B2-B025-4593-86AB-65151186337D}">
+    <text>no charts</text>
   </threadedComment>
   <threadedComment ref="D66" dT="2021-05-08T19:23:42.84" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{D1AD9B46-69A2-4F80-ADD4-0B51A5891E85}">
     <text>not works lists</text>
@@ -1495,47 +1628,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H98" sqref="H98"/>
+      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D1" s="14"/>
       <c r="E1" s="14" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F1" s="14"/>
       <c r="G1" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1544,22 +1677,22 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1568,85 +1701,85 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>115</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
@@ -1655,278 +1788,284 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
+      <c r="D14" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="4"/>
@@ -1935,12 +2074,12 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="4"/>
@@ -1949,88 +2088,92 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
+      <c r="D32" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="4"/>
@@ -2039,634 +2182,652 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="4"/>
+      <c r="D38" s="10" t="s">
+        <v>98</v>
+      </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="4"/>
+      <c r="D39" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
+      <c r="D40" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
+      <c r="D41" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="4"/>
+      <c r="D42" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49" s="5"/>
-      <c r="D49" s="4"/>
+      <c r="D49" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50" s="5"/>
-      <c r="D50" s="4"/>
+      <c r="D50" s="11" t="s">
+        <v>98</v>
+      </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54" s="5"/>
-      <c r="D54" s="4"/>
+      <c r="D54" s="12" t="s">
+        <v>98</v>
+      </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="12" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="10" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C69" s="5"/>
-      <c r="D69" s="4"/>
+      <c r="D69" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="4"/>
@@ -2675,33 +2836,33 @@
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -2709,243 +2870,245 @@
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C77" s="5"/>
-      <c r="D77" s="4"/>
+      <c r="D77" s="12" t="s">
+        <v>105</v>
+      </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -2953,102 +3116,102 @@
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="9" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="7"/>
       <c r="B97" s="7">
         <f>COUNTA(B3:B96)</f>
         <v>94</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D97" s="8">
         <f>COUNTIF(D3:D96,"identic")/$B$97</f>
-        <v>0.69148936170212771</v>
+        <v>0.81914893617021278</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="8">
@@ -3061,15 +3224,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D98" s="8">
         <f>COUNTA(D3:D96)/$B$97</f>
-        <v>0.76595744680851063</v>
+        <v>0.92553191489361697</v>
       </c>
       <c r="E98" s="7"/>
       <c r="F98" s="8">
@@ -3082,18 +3245,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H96" xr:uid="{CDCCD882-7221-41A5-A62B-B8C394BAD9F6}"/>
+  <autoFilter ref="A2:H96"/>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:D1"/>

</xml_diff>

<commit_message>
GKv3 (EtoForms): Improving of compatibility (2)
</commit_message>
<xml_diff>
--- a/dev_info/gk_compatibility_matrix.xlsx
+++ b/dev_info/gk_compatibility_matrix.xlsx
@@ -35,11 +35,15 @@
     <author>tc={B204A590-8F59-45C2-AF46-0C451D79A7F2}</author>
     <author>tc={FC38DB41-2593-4AE3-890A-83FAE8D7361F}</author>
     <author>tc={CABCC935-D353-49C6-BF7B-26945C3B7EEC}</author>
+    <author>Norseman</author>
     <author>tc={4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}</author>
     <author>tc={2E4E5FAA-8920-4E1C-B04E-22732D846631}</author>
+    <author>tc={2E4E5FAA-8920-4E1D-B04E-22732D846631}</author>
     <author>tc={08B0E8B2-B025-4593-86AB-65151186337D}</author>
     <author>tc={D1AD9B46-69A2-4F80-ADD4-0B51A5891E85}</author>
     <author>tc={BD118A23-46B1-45EB-A479-612E3372B34F}</author>
+    <author>tc={34F4FF22-A13C-482B-B521-D1FCFDCF8C10}</author>
+    <author>tc={D1AD9B46-69A2-4F81-ADD4-0B51A5891E85}</author>
   </authors>
   <commentList>
     <comment ref="D6" authorId="0">
@@ -117,7 +121,35 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="5">
+    <comment ref="D26" authorId="5">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>without map</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D27" authorId="5">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>without map</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D32" authorId="6">
       <text>
         <r>
           <rPr>
@@ -132,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D38" authorId="6">
+    <comment ref="D38" authorId="7">
       <text>
         <r>
           <rPr>
@@ -143,11 +175,11 @@
             <charset val="204"/>
             <scheme val="minor"/>
           </rPr>
-          <t>dialog scale inaccuracy</t>
+          <t>other inaccuracies</t>
         </r>
       </text>
     </comment>
-    <comment ref="D51" authorId="6">
+    <comment ref="D51" authorId="8">
       <text>
         <r>
           <rPr>
@@ -162,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D54" authorId="7">
+    <comment ref="D54" authorId="9">
       <text>
         <r>
           <rPr>
@@ -177,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D66" authorId="8">
+    <comment ref="D66" authorId="10">
       <text>
         <r>
           <rPr>
@@ -192,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D68" authorId="9">
+    <comment ref="D68" authorId="11">
       <text>
         <r>
           <rPr>
@@ -207,7 +239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D77" authorId="8">
+    <comment ref="D74" authorId="12">
       <text>
         <r>
           <rPr>
@@ -218,7 +250,22 @@
             <charset val="204"/>
             <scheme val="minor"/>
           </rPr>
-          <t>not works slidepanel</t>
+          <t>many errors and dont work sorting</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D77" authorId="13">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="204"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>not work slidepanel</t>
         </r>
       </text>
     </comment>
@@ -227,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="117">
   <si>
     <t>Module</t>
   </si>
@@ -518,9 +565,6 @@
   </si>
   <si>
     <t>GKUI\Components\ObservableExtList.cs</t>
-  </si>
-  <si>
-    <t>GKUI\Components\GKMenuItem.cs</t>
   </si>
   <si>
     <t>identic</t>
@@ -623,6 +667,9 @@
   <si>
     <t>GKUI\Platform\EtoAppHost.cs</t>
   </si>
+  <si>
+    <t>GKUI\Platform\MenuItemEx.cs</t>
+  </si>
 </sst>
 </file>
 
@@ -631,7 +678,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,6 +838,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="40">
@@ -1612,7 +1666,10 @@
   <threadedComment ref="D32" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}">
     <text>require toolbar's combobox and dropdownbtn</text>
   </threadedComment>
-  <threadedComment ref="D51" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{2E4E5FAA-8920-4E1C-B04E-22732D846631}">
+  <threadedComment ref="D38" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{2E4E5FAA-8920-4E1C-B04E-22732D846631}">
+    <text>other inaccuracies</text>
+  </threadedComment>
+  <threadedComment ref="D51" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{2E4E5FAA-8920-4E1D-B04E-22732D846631}">
     <text>first image not fitted to window</text>
   </threadedComment>
   <threadedComment ref="D54" dT="2021-05-08T19:23:42.84" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{08B0E8B2-B025-4593-86AB-65151186337D}">
@@ -1624,6 +1681,12 @@
   <threadedComment ref="D68" dT="2021-05-07T19:42:23.30" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{BD118A23-46B1-45EB-A479-612E3372B34F}">
     <text>lines without arrow's caps</text>
   </threadedComment>
+  <threadedComment ref="D74" dT="2021-05-12T13:41:55.52" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{34F4FF22-A13C-482B-B521-D1FCFDCF8C10}">
+    <text>many errors and dont work sorting</text>
+  </threadedComment>
+  <threadedComment ref="D77" dT="2021-05-08T19:23:42.84" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{D1AD9B46-69A2-4F81-ADD4-0B51A5891E85}">
+    <text>not work slidepanel</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -1632,20 +1695,20 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1677,19 +1740,19 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
@@ -1701,7 +1764,7 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1713,13 +1776,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1735,7 +1798,7 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1751,7 +1814,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -1767,7 +1830,7 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -1782,7 +1845,9 @@
         <v>9</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
+      <c r="D8" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -1797,7 +1862,7 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -1813,7 +1878,7 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -1829,7 +1894,7 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -1845,7 +1910,7 @@
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -1861,7 +1926,7 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -1877,7 +1942,7 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -1893,7 +1958,7 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1909,7 +1974,7 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -1925,7 +1990,7 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1941,7 +2006,7 @@
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
@@ -1957,7 +2022,7 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -1973,7 +2038,7 @@
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1989,7 +2054,7 @@
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -2005,7 +2070,7 @@
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
@@ -2021,7 +2086,7 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -2037,7 +2102,7 @@
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -2053,7 +2118,7 @@
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
@@ -2068,7 +2133,9 @@
         <v>27</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
+      <c r="D26" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -2082,7 +2149,9 @@
         <v>28</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
+      <c r="D27" s="10" t="s">
+        <v>97</v>
+      </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
@@ -2097,7 +2166,7 @@
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -2113,7 +2182,7 @@
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -2129,7 +2198,7 @@
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -2145,7 +2214,7 @@
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -2161,7 +2230,7 @@
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2176,7 +2245,9 @@
         <v>34</v>
       </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="4"/>
+      <c r="D33" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -2191,7 +2262,7 @@
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -2207,7 +2278,7 @@
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -2223,7 +2294,7 @@
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -2239,7 +2310,7 @@
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -2255,7 +2326,7 @@
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -2271,7 +2342,7 @@
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -2287,7 +2358,7 @@
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -2303,7 +2374,7 @@
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -2319,7 +2390,7 @@
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -2335,7 +2406,7 @@
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -2351,7 +2422,7 @@
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -2367,7 +2438,7 @@
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -2383,7 +2454,7 @@
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -2399,7 +2470,7 @@
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
@@ -2415,7 +2486,7 @@
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
@@ -2431,7 +2502,7 @@
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
@@ -2447,7 +2518,7 @@
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
@@ -2463,7 +2534,7 @@
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
@@ -2479,7 +2550,7 @@
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
@@ -2495,7 +2566,7 @@
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -2511,7 +2582,7 @@
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2527,7 +2598,7 @@
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2543,7 +2614,7 @@
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2559,7 +2630,7 @@
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -2575,7 +2646,7 @@
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2591,7 +2662,7 @@
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -2607,7 +2678,7 @@
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -2623,7 +2694,7 @@
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -2639,7 +2710,7 @@
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -2655,7 +2726,7 @@
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -2671,7 +2742,7 @@
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -2687,7 +2758,7 @@
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -2703,7 +2774,7 @@
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
@@ -2719,7 +2790,7 @@
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
@@ -2735,7 +2806,7 @@
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
@@ -2751,7 +2822,7 @@
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -2767,7 +2838,7 @@
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
@@ -2783,7 +2854,7 @@
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
@@ -2799,7 +2870,7 @@
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -2815,7 +2886,7 @@
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
@@ -2830,7 +2901,9 @@
         <v>75</v>
       </c>
       <c r="C74" s="5"/>
-      <c r="D74" s="4"/>
+      <c r="D74" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -2847,7 +2920,7 @@
         <v>95</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -2862,9 +2935,11 @@
         <v>95</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D76" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>97</v>
+      </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
@@ -2879,7 +2954,7 @@
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
@@ -2895,7 +2970,7 @@
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
@@ -2911,7 +2986,7 @@
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
@@ -2927,7 +3002,7 @@
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
@@ -2943,7 +3018,7 @@
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
@@ -2959,7 +3034,7 @@
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
@@ -2975,7 +3050,7 @@
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
@@ -2991,7 +3066,7 @@
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
@@ -3007,7 +3082,7 @@
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
@@ -3041,7 +3116,7 @@
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
@@ -3057,7 +3132,7 @@
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
@@ -3069,13 +3144,13 @@
         <v>3</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
@@ -3087,13 +3162,13 @@
         <v>3</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
@@ -3108,51 +3183,53 @@
         <v>95</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D91" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>104</v>
+      </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>3</v>
       </c>
@@ -3161,7 +3238,7 @@
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
@@ -3177,7 +3254,7 @@
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
@@ -3193,7 +3270,7 @@
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
@@ -3207,11 +3284,11 @@
         <v>94</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D97" s="8">
         <f>COUNTIF(D3:D96,"identic")/$B$97</f>
-        <v>0.81914893617021278</v>
+        <v>0.86170212765957444</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="8">
@@ -3228,11 +3305,11 @@
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D98" s="8">
         <f>COUNTA(D3:D96)/$B$97</f>
-        <v>0.92553191489361697</v>
+        <v>1</v>
       </c>
       <c r="E98" s="7"/>
       <c r="F98" s="8">
@@ -3247,12 +3324,12 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GKv3 (EtoForms): Improving of compatibility (3)
</commit_message>
<xml_diff>
--- a/dev_info/gk_compatibility_matrix.xlsx
+++ b/dev_info/gk_compatibility_matrix.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Compatibility Matrix" sheetId="2" r:id="rId1"/>
+    <sheet name="Linux(Mono) Status" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Compatibility Matrix'!$A$2:$H$96</definedName>
@@ -33,14 +34,11 @@
     <author>tc={0C8C2A0A-09FB-4B08-999F-C16384413ED6}</author>
     <author>tc={03199625-ADA0-4544-BEED-2EC70A7B7558}</author>
     <author>tc={B204A590-8F59-45C2-AF46-0C451D79A7F2}</author>
-    <author>tc={FC38DB41-2593-4AE3-890A-83FAE8D7361F}</author>
     <author>tc={CABCC935-D353-49C6-BF7B-26945C3B7EEC}</author>
     <author>Norseman</author>
     <author>tc={4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}</author>
-    <author>tc={2E4E5FAA-8920-4E1C-B04E-22732D846631}</author>
     <author>tc={2E4E5FAA-8920-4E1D-B04E-22732D846631}</author>
     <author>tc={08B0E8B2-B025-4593-86AB-65151186337D}</author>
-    <author>tc={D1AD9B46-69A2-4F80-ADD4-0B51A5891E85}</author>
     <author>tc={BD118A23-46B1-45EB-A479-612E3372B34F}</author>
     <author>tc={34F4FF22-A13C-482B-B521-D1FCFDCF8C10}</author>
     <author>tc={D1AD9B46-69A2-4F81-ADD4-0B51A5891E85}</author>
@@ -91,22 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="3">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>many small inaccuracies</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D20" authorId="4">
+    <comment ref="D20" authorId="3">
       <text>
         <r>
           <rPr>
@@ -121,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D26" authorId="5">
+    <comment ref="D26" authorId="4">
       <text>
         <r>
           <rPr>
@@ -135,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D27" authorId="5">
+    <comment ref="D27" authorId="4">
       <text>
         <r>
           <rPr>
@@ -149,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D32" authorId="6">
+    <comment ref="D32" authorId="5">
       <text>
         <r>
           <rPr>
@@ -164,22 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D38" authorId="7">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>other inaccuracies</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D51" authorId="8">
+    <comment ref="D51" authorId="6">
       <text>
         <r>
           <rPr>
@@ -194,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D54" authorId="9">
+    <comment ref="D54" authorId="7">
       <text>
         <r>
           <rPr>
@@ -209,22 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D66" authorId="10">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>not works lists</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D68" authorId="11">
+    <comment ref="D68" authorId="8">
       <text>
         <r>
           <rPr>
@@ -239,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D74" authorId="12">
+    <comment ref="D74" authorId="9">
       <text>
         <r>
           <rPr>
@@ -254,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D77" authorId="13">
+    <comment ref="D77" authorId="10">
       <text>
         <r>
           <rPr>
@@ -273,8 +226,122 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Автор</author>
+  </authors>
+  <commentList>
+    <comment ref="D14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>ZSV: need refactoring and optimization</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>ZSV: It seems to work, but need massive testing</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>ZSV: WebBrowser does not work, it's frozen</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D41" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>ZSV: distortions</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="261">
   <si>
     <t>Module</t>
   </si>
@@ -670,6 +737,438 @@
   <si>
     <t>GKUI\Platform\MenuItemEx.cs</t>
   </si>
+  <si>
+    <t>№</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Comment (C#/Mono)</t>
+  </si>
+  <si>
+    <t>C#/Mono (2016)</t>
+  </si>
+  <si>
+    <t>C#/Eto (2017)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Basic functionality</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>Starting and closing the program</t>
+  </si>
+  <si>
+    <t>1.1.1</t>
+  </si>
+  <si>
+    <t>Running the second instance with the transfer of control to the first</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
+    <t>Logging</t>
+  </si>
+  <si>
+    <t>1.1.3</t>
+  </si>
+  <si>
+    <t>Sending of logs by default mail's client</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Database creation</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Closing the database</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>Loading the database</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Saving the database</t>
+  </si>
+  <si>
+    <t>1.5.1</t>
+  </si>
+  <si>
+    <t>Encrypted files</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>Loading and saving settings</t>
+  </si>
+  <si>
+    <t>1.7</t>
+  </si>
+  <si>
+    <t>Work of the lists of records (ListView)</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>Sorting lists</t>
+  </si>
+  <si>
+    <t>1.9</t>
+  </si>
+  <si>
+    <t>View hypertext of record's contents (HyperView)</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>Add, edit, and delete records</t>
+  </si>
+  <si>
+    <t>1.10.1</t>
+  </si>
+  <si>
+    <t>Work of all edit dialogs</t>
+  </si>
+  <si>
+    <t>1.11</t>
+  </si>
+  <si>
+    <t>Quick search</t>
+  </si>
+  <si>
+    <t>1.12</t>
+  </si>
+  <si>
+    <t>Filtration</t>
+  </si>
+  <si>
+    <t>1.13</t>
+  </si>
+  <si>
+    <t>Display and view all types of trees</t>
+  </si>
+  <si>
+    <t>1.14</t>
+  </si>
+  <si>
+    <t>Circle of ancestors / descendants</t>
+  </si>
+  <si>
+    <t>1.15</t>
+  </si>
+  <si>
+    <t>Pedigrees (html)</t>
+  </si>
+  <si>
+    <t>1.16</t>
+  </si>
+  <si>
+    <t>Pedigrees (rtf)</t>
+  </si>
+  <si>
+    <t>1.17</t>
+  </si>
+  <si>
+    <t>Pedigrees (pdf)</t>
+  </si>
+  <si>
+    <t>1.18</t>
+  </si>
+  <si>
+    <t>FamilyBook (pdf)</t>
+  </si>
+  <si>
+    <t>1.19</t>
+  </si>
+  <si>
+    <t>Maps</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>Statistics</t>
+  </si>
+  <si>
+    <t>1.21.1</t>
+  </si>
+  <si>
+    <t>Charts (line, bars)</t>
+  </si>
+  <si>
+    <t>1.21</t>
+  </si>
+  <si>
+    <t>Organizer</t>
+  </si>
+  <si>
+    <t>1.22</t>
+  </si>
+  <si>
+    <t>Slideshow</t>
+  </si>
+  <si>
+    <t>1.23</t>
+  </si>
+  <si>
+    <t>Scripts</t>
+  </si>
+  <si>
+    <t>1.24</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>Loading plugins</t>
+  </si>
+  <si>
+    <t>1.26</t>
+  </si>
+  <si>
+    <t>Window management (cascade, tile, etc)</t>
+  </si>
+  <si>
+    <t>deprecated</t>
+  </si>
+  <si>
+    <t>1.27</t>
+  </si>
+  <si>
+    <t>Help contents</t>
+  </si>
+  <si>
+    <t>1.28</t>
+  </si>
+  <si>
+    <t>Correct display of windows, scaling</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
+    <t>Switching languages</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>Manage lists (SheetList)</t>
+  </si>
+  <si>
+    <t>1.31</t>
+  </si>
+  <si>
+    <t>Progression</t>
+  </si>
+  <si>
+    <t>1.32</t>
+  </si>
+  <si>
+    <t>Icons of the main toolbar</t>
+  </si>
+  <si>
+    <t>1.33</t>
+  </si>
+  <si>
+    <t>File properties and selection file language</t>
+  </si>
+  <si>
+    <t>1.34</t>
+  </si>
+  <si>
+    <t>Custom toolbars (in controls and panels)</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>Exporting data to Excel</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>Compare databases</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>Merge databases</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>Split databases</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>Merge duplicates</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>Check connectivity and logarithmic graph of fragmentation</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>Check databases</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>Search for patriarchs</t>
+  </si>
+  <si>
+    <t>2.8.1</t>
+  </si>
+  <si>
+    <t>Displaying the relationship graph for patriarchs</t>
+  </si>
+  <si>
+    <t>ArborGVT freezes</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>Manage places</t>
+  </si>
+  <si>
+    <t>2.10</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Advanced features (plugins)</t>
+  </si>
+  <si>
+    <t>3.1</t>
+  </si>
+  <si>
+    <t>Calculator</t>
+  </si>
+  <si>
+    <t>Drag does not work</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>Stream input</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>ImagesViewer</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>Game of Life</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>Names Book</t>
+  </si>
+  <si>
+    <t>3.7</t>
+  </si>
+  <si>
+    <t>Import of pedigrees</t>
+  </si>
+  <si>
+    <t>Works itself import and formats (csv, txt), not available doc, xls.</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>Plugin example</t>
+  </si>
+  <si>
+    <t>3.9</t>
+  </si>
+  <si>
+    <t>Full text search</t>
+  </si>
+  <si>
+    <t>Difficult Xapian-extdepend; the plugin is not promising and frozen.</t>
+  </si>
+  <si>
+    <t>3.10</t>
+  </si>
+  <si>
+    <t>Time line</t>
+  </si>
+  <si>
+    <t>3.11</t>
+  </si>
+  <si>
+    <t>3D Tree Visualization</t>
+  </si>
+  <si>
+    <t>Difficult OpenGL-extdepend; the plugin is not promising and frozen.</t>
+  </si>
+  <si>
+    <t>3.12</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Distribution for Linux (Debian/Ubuntu)</t>
+  </si>
 </sst>
 </file>
 
@@ -678,7 +1177,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -846,8 +1345,37 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1069,8 +1597,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1200,8 +1746,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1245,8 +1815,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1286,8 +1858,62 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="43" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="34" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="16" fillId="0" borderId="10" xfId="43" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="43" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="38" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="40" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="43" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="39" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="36" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="41" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="41" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="41" borderId="12" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="20" fillId="0" borderId="10" xfId="43" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="42" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="20" fillId="35" borderId="10" xfId="43" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="16" fillId="35" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="20% - Акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1324,10 +1950,12 @@
     <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный 2" xfId="43"/>
     <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Процентный" xfId="42" builtinId="5"/>
+    <cellStyle name="Процентный 2" xfId="44"/>
     <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
@@ -1694,9 +2322,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,7 +2561,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1941,7 +2569,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="11" t="s">
         <v>97</v>
       </c>
       <c r="E14" s="4"/>
@@ -1949,7 +2577,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1965,7 +2593,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -1981,7 +2609,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1997,7 +2625,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -2013,7 +2641,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2029,7 +2657,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -2045,7 +2673,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -2061,7 +2689,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -2077,7 +2705,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
@@ -2093,7 +2721,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -2109,7 +2737,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
@@ -2125,7 +2753,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -2133,7 +2761,7 @@
         <v>27</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E26" s="4"/>
@@ -2141,7 +2769,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
@@ -2149,7 +2777,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="12" t="s">
         <v>97</v>
       </c>
       <c r="E27" s="4"/>
@@ -2157,7 +2785,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -2173,7 +2801,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
@@ -2189,7 +2817,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
@@ -2205,7 +2833,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
@@ -2221,7 +2849,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
@@ -2237,7 +2865,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
@@ -2253,7 +2881,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
@@ -2269,7 +2897,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>2</v>
       </c>
@@ -2285,7 +2913,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
@@ -2301,7 +2929,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
@@ -2317,7 +2945,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>2</v>
       </c>
@@ -2325,7 +2953,7 @@
         <v>39</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="11" t="s">
         <v>97</v>
       </c>
       <c r="E38" s="4"/>
@@ -2333,7 +2961,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
@@ -2349,7 +2977,7 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
@@ -2365,7 +2993,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>2</v>
       </c>
@@ -2381,7 +3009,7 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
@@ -2397,7 +3025,7 @@
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -2413,7 +3041,7 @@
       <c r="G43" s="4"/>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
@@ -2429,7 +3057,7 @@
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>2</v>
       </c>
@@ -2445,7 +3073,7 @@
       <c r="G45" s="4"/>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>2</v>
       </c>
@@ -2461,7 +3089,7 @@
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>2</v>
       </c>
@@ -2477,7 +3105,7 @@
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>2</v>
       </c>
@@ -2493,7 +3121,7 @@
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>2</v>
       </c>
@@ -2509,7 +3137,7 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>2</v>
       </c>
@@ -2525,7 +3153,7 @@
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
@@ -2541,7 +3169,7 @@
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
@@ -2557,7 +3185,7 @@
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
@@ -2573,7 +3201,7 @@
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>2</v>
       </c>
@@ -2589,7 +3217,7 @@
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
     </row>
-    <row r="55" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>2</v>
       </c>
@@ -2605,7 +3233,7 @@
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
     </row>
-    <row r="56" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>2</v>
       </c>
@@ -2621,7 +3249,7 @@
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
     </row>
-    <row r="57" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
@@ -2637,7 +3265,7 @@
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
     </row>
-    <row r="58" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>2</v>
       </c>
@@ -2653,7 +3281,7 @@
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>2</v>
       </c>
@@ -2669,7 +3297,7 @@
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
     </row>
-    <row r="60" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
@@ -2685,7 +3313,7 @@
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
     </row>
-    <row r="61" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>2</v>
       </c>
@@ -2701,7 +3329,7 @@
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
     </row>
-    <row r="62" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>2</v>
       </c>
@@ -2717,7 +3345,7 @@
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
     </row>
-    <row r="63" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>2</v>
       </c>
@@ -2733,7 +3361,7 @@
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
     </row>
-    <row r="64" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>2</v>
       </c>
@@ -2749,7 +3377,7 @@
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
     </row>
-    <row r="65" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>2</v>
       </c>
@@ -2765,7 +3393,7 @@
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
     </row>
-    <row r="66" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>2</v>
       </c>
@@ -2773,7 +3401,7 @@
         <v>67</v>
       </c>
       <c r="C66" s="5"/>
-      <c r="D66" s="12" t="s">
+      <c r="D66" s="11" t="s">
         <v>97</v>
       </c>
       <c r="E66" s="4"/>
@@ -2781,7 +3409,7 @@
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
     </row>
-    <row r="67" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
@@ -2797,7 +3425,7 @@
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
     </row>
-    <row r="68" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>3</v>
       </c>
@@ -2813,7 +3441,7 @@
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
     </row>
-    <row r="69" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>3</v>
       </c>
@@ -2821,7 +3449,7 @@
         <v>70</v>
       </c>
       <c r="C69" s="5"/>
-      <c r="D69" s="11" t="s">
+      <c r="D69" s="10" t="s">
         <v>104</v>
       </c>
       <c r="E69" s="4"/>
@@ -2829,7 +3457,7 @@
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
     </row>
-    <row r="70" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>3</v>
       </c>
@@ -2837,15 +3465,15 @@
         <v>71</v>
       </c>
       <c r="C70" s="5"/>
-      <c r="D70" s="9" t="s">
-        <v>100</v>
+      <c r="D70" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
     </row>
-    <row r="71" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>3</v>
       </c>
@@ -2861,7 +3489,7 @@
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
     </row>
-    <row r="72" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>3</v>
       </c>
@@ -2877,7 +3505,7 @@
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
     </row>
-    <row r="73" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>3</v>
       </c>
@@ -2893,7 +3521,7 @@
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
     </row>
-    <row r="74" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>3</v>
       </c>
@@ -2945,7 +3573,7 @@
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
     </row>
-    <row r="77" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>3</v>
       </c>
@@ -2961,7 +3589,7 @@
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
     </row>
-    <row r="78" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>3</v>
       </c>
@@ -2977,7 +3605,7 @@
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
     </row>
-    <row r="79" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>3</v>
       </c>
@@ -2993,7 +3621,7 @@
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
     </row>
-    <row r="80" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>3</v>
       </c>
@@ -3009,7 +3637,7 @@
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
     </row>
-    <row r="81" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>3</v>
       </c>
@@ -3025,7 +3653,7 @@
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
     </row>
-    <row r="82" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
@@ -3041,7 +3669,7 @@
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
     </row>
-    <row r="83" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
@@ -3057,7 +3685,7 @@
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
     </row>
-    <row r="84" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
@@ -3073,7 +3701,7 @@
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
     </row>
-    <row r="85" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
@@ -3107,7 +3735,7 @@
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
     </row>
-    <row r="87" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>3</v>
       </c>
@@ -3123,7 +3751,7 @@
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
     </row>
-    <row r="88" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>3</v>
       </c>
@@ -3139,7 +3767,7 @@
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
     </row>
-    <row r="89" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>3</v>
       </c>
@@ -3157,7 +3785,7 @@
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
     </row>
-    <row r="90" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>3</v>
       </c>
@@ -3193,7 +3821,7 @@
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
     </row>
-    <row r="92" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>3</v>
       </c>
@@ -3211,7 +3839,7 @@
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
     </row>
-    <row r="93" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>3</v>
       </c>
@@ -3229,7 +3857,7 @@
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
     </row>
-    <row r="94" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>3</v>
       </c>
@@ -3288,7 +3916,7 @@
       </c>
       <c r="D97" s="8">
         <f>COUNTIF(D3:D96,"identic")/$B$97</f>
-        <v>0.86170212765957444</v>
+        <v>0.87234042553191493</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="8">
@@ -3344,4 +3972,1058 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="16"/>
+    <col min="2" max="2" width="62" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="62.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="24">
+        <v>1</v>
+      </c>
+      <c r="D4" s="24">
+        <v>1</v>
+      </c>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="24">
+        <v>1</v>
+      </c>
+      <c r="D5" s="26">
+        <v>0</v>
+      </c>
+      <c r="E5" s="27"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="24">
+        <v>1</v>
+      </c>
+      <c r="D6" s="24">
+        <v>1</v>
+      </c>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="24">
+        <v>1</v>
+      </c>
+      <c r="D7" s="24">
+        <v>1</v>
+      </c>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="24">
+        <v>1</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1</v>
+      </c>
+      <c r="E8" s="28"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" s="24">
+        <v>1</v>
+      </c>
+      <c r="D9" s="24">
+        <v>1</v>
+      </c>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="24">
+        <v>1</v>
+      </c>
+      <c r="D10" s="24">
+        <v>1</v>
+      </c>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="24">
+        <v>1</v>
+      </c>
+      <c r="D11" s="24">
+        <v>1</v>
+      </c>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C12" s="24">
+        <v>1</v>
+      </c>
+      <c r="D12" s="24">
+        <v>1</v>
+      </c>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="24">
+        <v>1</v>
+      </c>
+      <c r="D13" s="24">
+        <v>1</v>
+      </c>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="24">
+        <v>1</v>
+      </c>
+      <c r="D14" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="E14" s="28"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="24">
+        <v>1</v>
+      </c>
+      <c r="D15" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="24">
+        <v>1</v>
+      </c>
+      <c r="D16" s="24">
+        <v>1</v>
+      </c>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="24">
+        <v>1</v>
+      </c>
+      <c r="D17" s="26">
+        <v>0</v>
+      </c>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="24">
+        <v>1</v>
+      </c>
+      <c r="D18" s="26">
+        <v>0</v>
+      </c>
+      <c r="E18" s="28"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="24">
+        <v>1</v>
+      </c>
+      <c r="D19" s="24">
+        <v>1</v>
+      </c>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="24">
+        <v>1</v>
+      </c>
+      <c r="D20" s="30">
+        <v>0</v>
+      </c>
+      <c r="E20" s="28"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="24">
+        <v>1</v>
+      </c>
+      <c r="D21" s="24">
+        <v>1</v>
+      </c>
+      <c r="E21" s="28"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="C22" s="24">
+        <v>1</v>
+      </c>
+      <c r="D22" s="24">
+        <v>1</v>
+      </c>
+      <c r="E22" s="28"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="24">
+        <v>1</v>
+      </c>
+      <c r="D23" s="24">
+        <v>1</v>
+      </c>
+      <c r="E23" s="28"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" s="24">
+        <v>1</v>
+      </c>
+      <c r="D24" s="24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="28"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" s="24">
+        <v>1</v>
+      </c>
+      <c r="D25" s="24">
+        <v>1</v>
+      </c>
+      <c r="E25" s="28"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="31"/>
+      <c r="D26" s="26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="28"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="26">
+        <v>0</v>
+      </c>
+      <c r="E27" s="28"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C28" s="24">
+        <v>1</v>
+      </c>
+      <c r="D28" s="24">
+        <v>1</v>
+      </c>
+      <c r="E28" s="28"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="24">
+        <v>1</v>
+      </c>
+      <c r="D29" s="30">
+        <v>0</v>
+      </c>
+      <c r="E29" s="28"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C30" s="24">
+        <v>1</v>
+      </c>
+      <c r="D30" s="24">
+        <v>1</v>
+      </c>
+      <c r="E30" s="28"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" s="24">
+        <v>1</v>
+      </c>
+      <c r="D31" s="24">
+        <v>1</v>
+      </c>
+      <c r="E31" s="28"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="24">
+        <v>1</v>
+      </c>
+      <c r="D32" s="24">
+        <v>1</v>
+      </c>
+      <c r="E32" s="28"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="24">
+        <v>1</v>
+      </c>
+      <c r="D33" s="24">
+        <v>1</v>
+      </c>
+      <c r="E33" s="28"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="C34" s="24">
+        <v>1</v>
+      </c>
+      <c r="D34" s="24">
+        <v>1</v>
+      </c>
+      <c r="E34" s="28"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="33"/>
+      <c r="E35" s="28"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36" s="24">
+        <v>1</v>
+      </c>
+      <c r="D36" s="24">
+        <v>1</v>
+      </c>
+      <c r="E36" s="28"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C37" s="24">
+        <v>1</v>
+      </c>
+      <c r="D37" s="30">
+        <v>0</v>
+      </c>
+      <c r="E37" s="28"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B38" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="C38" s="24">
+        <v>1</v>
+      </c>
+      <c r="D38" s="24">
+        <v>1</v>
+      </c>
+      <c r="E38" s="28"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="C39" s="24">
+        <v>1</v>
+      </c>
+      <c r="D39" s="30">
+        <v>0</v>
+      </c>
+      <c r="E39" s="28"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="B40" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="C40" s="24">
+        <v>1</v>
+      </c>
+      <c r="D40" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="E40" s="28"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="C41" s="24">
+        <v>1</v>
+      </c>
+      <c r="D41" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="E41" s="28"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="B42" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="C42" s="24">
+        <v>1</v>
+      </c>
+      <c r="D42" s="24">
+        <v>1</v>
+      </c>
+      <c r="E42" s="28"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="C43" s="24">
+        <v>1</v>
+      </c>
+      <c r="D43" s="30">
+        <v>0</v>
+      </c>
+      <c r="E43" s="28"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="22"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="28"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>209</v>
+      </c>
+      <c r="C46" s="24">
+        <v>1</v>
+      </c>
+      <c r="D46" s="24">
+        <v>1</v>
+      </c>
+      <c r="E46" s="28"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" s="24">
+        <v>1</v>
+      </c>
+      <c r="D47" s="24">
+        <v>1</v>
+      </c>
+      <c r="E47" s="28"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="24">
+        <v>1</v>
+      </c>
+      <c r="D48" s="24">
+        <v>1</v>
+      </c>
+      <c r="E48" s="28"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="C49" s="24">
+        <v>1</v>
+      </c>
+      <c r="D49" s="24">
+        <v>1</v>
+      </c>
+      <c r="E49" s="28"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B50" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="C50" s="24">
+        <v>1</v>
+      </c>
+      <c r="D50" s="24">
+        <v>1</v>
+      </c>
+      <c r="E50" s="28"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="C51" s="24">
+        <v>1</v>
+      </c>
+      <c r="D51" s="24">
+        <v>1</v>
+      </c>
+      <c r="E51" s="28"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" s="23" t="s">
+        <v>221</v>
+      </c>
+      <c r="C52" s="24">
+        <v>1</v>
+      </c>
+      <c r="D52" s="24">
+        <v>1</v>
+      </c>
+      <c r="E52" s="28"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C53" s="24">
+        <v>1</v>
+      </c>
+      <c r="D53" s="24">
+        <v>1</v>
+      </c>
+      <c r="E53" s="28"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="B54" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="C54" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="D54" s="24">
+        <v>1</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="C55" s="24">
+        <v>1</v>
+      </c>
+      <c r="D55" s="24">
+        <v>1</v>
+      </c>
+      <c r="E55" s="28"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="B56" s="28"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="28"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="21"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="B58" s="23" t="s">
+        <v>233</v>
+      </c>
+      <c r="C58" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="D58" s="30">
+        <v>0</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="B59" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="C59" s="24">
+        <v>1</v>
+      </c>
+      <c r="D59" s="26">
+        <v>0</v>
+      </c>
+      <c r="E59" s="28"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="B60" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="C60" s="24">
+        <v>1</v>
+      </c>
+      <c r="D60" s="26">
+        <v>0</v>
+      </c>
+      <c r="E60" s="28"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B61" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="C61" s="24">
+        <v>1</v>
+      </c>
+      <c r="D61" s="26">
+        <v>0</v>
+      </c>
+      <c r="E61" s="28"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="B62" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="C62" s="24">
+        <v>1</v>
+      </c>
+      <c r="D62" s="26">
+        <v>0</v>
+      </c>
+      <c r="E62" s="28"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B63" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="C63" s="24">
+        <v>1</v>
+      </c>
+      <c r="D63" s="26">
+        <v>0</v>
+      </c>
+      <c r="E63" s="28"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="B64" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="C64" s="29">
+        <v>0.75</v>
+      </c>
+      <c r="D64" s="26">
+        <v>0</v>
+      </c>
+      <c r="E64" s="28" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="B65" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="C65" s="24">
+        <v>1</v>
+      </c>
+      <c r="D65" s="26">
+        <v>0</v>
+      </c>
+      <c r="E65" s="28"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="B66" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="C66" s="31"/>
+      <c r="D66" s="31"/>
+      <c r="E66" s="28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="B67" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="C67" s="24">
+        <v>1</v>
+      </c>
+      <c r="D67" s="26">
+        <v>0</v>
+      </c>
+      <c r="E67" s="28"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="B68" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="28" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="35" t="s">
+        <v>258</v>
+      </c>
+      <c r="B69" s="28"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="28"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C70" s="24">
+        <v>1</v>
+      </c>
+      <c r="D70" s="26">
+        <v>0</v>
+      </c>
+      <c r="E70" s="21"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="38"/>
+      <c r="B71" s="39"/>
+      <c r="C71" s="40">
+        <f>AVERAGE(C3:C70)</f>
+        <v>0.98947368421052628</v>
+      </c>
+      <c r="D71" s="40">
+        <f>AVERAGE(D3:D70)</f>
+        <v>0.63813559322033897</v>
+      </c>
+      <c r="E71" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="C35:D35"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
GKv2/GKv3 compatibility fixes (1)
</commit_message>
<xml_diff>
--- a/dev_info/gk_compatibility_matrix.xlsx
+++ b/dev_info/gk_compatibility_matrix.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKS\shared\gkdev\GEDKeeper\dev_info\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB49238-4385-467E-B10C-B565134B60E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compatibility Matrix" sheetId="2" r:id="rId1"/>
     <sheet name="Linux(Mono) Status" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Compatibility Matrix'!$A$2:$H$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Compatibility Matrix'!$A$2:$F$96</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -22,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,13 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={0C8C2A0A-09FB-4B08-999F-C16384413ED6}</author>
     <author>tc={03199625-ADA0-4544-BEED-2EC70A7B7558}</author>
     <author>tc={B204A590-8F59-45C2-AF46-0C451D79A7F2}</author>
     <author>tc={CABCC935-D353-49C6-BF7B-26945C3B7EEC}</author>
-    <author>Norseman</author>
     <author>tc={4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}</author>
     <author>tc={2E4E5FAA-8920-4E1D-B04E-22732D846631}</author>
     <author>tc={08B0E8B2-B025-4593-86AB-65151186337D}</author>
@@ -44,182 +50,84 @@
     <author>tc={D1AD9B46-69A2-4F81-ADD4-0B51A5891E85}</author>
   </authors>
   <commentList>
-    <comment ref="D6" authorId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>coordinates from ScrollPanel, unify</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    coordinates from ScrollPanel, unify</t>
       </text>
     </comment>
-    <comment ref="D7" authorId="1">
+    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>no metafiles</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    no metafiles</t>
       </text>
     </comment>
-    <comment ref="D10" authorId="2">
+    <comment ref="D10" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>many small inaccuracies</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    many small inaccuracies</t>
       </text>
     </comment>
-    <comment ref="D20" authorId="3">
+    <comment ref="D20" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>no dragdrop</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    no dragdrop</t>
       </text>
     </comment>
-    <comment ref="D26" authorId="4">
+    <comment ref="D32" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>without map</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    require toolbar's combobox and dropdownbtn</t>
       </text>
     </comment>
-    <comment ref="D27" authorId="4">
+    <comment ref="D51" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>without map</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    first image not fitted to window</t>
       </text>
     </comment>
-    <comment ref="D32" authorId="5">
+    <comment ref="D54" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>require toolbar's combobox and dropdownbtn</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    no charts</t>
       </text>
     </comment>
-    <comment ref="D51" authorId="6">
+    <comment ref="D68" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>first image not fitted to window</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    lines without arrow's caps</t>
       </text>
     </comment>
-    <comment ref="D54" authorId="7">
+    <comment ref="D74" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>no charts</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    many errors and dont work sorting</t>
       </text>
     </comment>
-    <comment ref="D68" authorId="8">
+    <comment ref="D77" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>lines without arrow's caps</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D74" authorId="9">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>many errors and dont work sorting</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D77" authorId="10">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>not work slidepanel</t>
-        </r>
+        <t>[Цепочка примечаний]
+Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
+Комментарий:
+    not work slidepanel</t>
       </text>
     </comment>
   </commentList>
@@ -227,12 +135,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="D14" authorId="0">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -258,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D15" authorId="0">
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -284,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0">
+    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -310,38 +218,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="D41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t>ZSV: distortions</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="260">
   <si>
     <t>Module</t>
   </si>
@@ -623,9 +505,6 @@
   </si>
   <si>
     <t>GKvX (Xamarin)</t>
-  </si>
-  <si>
-    <t>GKvU (UWP)</t>
   </si>
   <si>
     <t>—</t>
@@ -1173,11 +1052,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1337,13 +1216,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1815,10 +1687,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1855,13 +1727,7 @@
     <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="43"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="43"/>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1870,18 +1736,18 @@
     <xf numFmtId="2" fontId="16" fillId="34" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="16" fillId="0" borderId="10" xfId="43" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="43" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="16" fillId="38" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="16" fillId="40" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="43" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="43" applyBorder="1"/>
     <xf numFmtId="2" fontId="16" fillId="39" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1891,47 +1757,56 @@
     <xf numFmtId="2" fontId="16" fillId="41" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="0" borderId="10" xfId="43" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="42" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="35" borderId="10" xfId="43" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="16" fillId="35" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="16" fillId="41" borderId="11" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="41" borderId="12" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="20" fillId="0" borderId="10" xfId="43" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="42" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="10" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="20" fillId="35" borderId="10" xfId="43" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="43" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="16" fillId="35" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="42" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
-    <cellStyle name="20% - Акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -1950,12 +1825,12 @@
     <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="43"/>
+    <cellStyle name="Обычный 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Процентный" xfId="42" builtinId="5"/>
-    <cellStyle name="Процентный 2" xfId="44"/>
+    <cellStyle name="Процентный 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
     <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
@@ -2268,7 +2143,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2285,26 +2160,17 @@
   <threadedComment ref="D10" dT="2021-05-08T22:17:18.54" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{B204A590-8F59-45C2-AF46-0C451D79A7F2}">
     <text>many small inaccuracies</text>
   </threadedComment>
-  <threadedComment ref="D14" dT="2021-05-08T22:17:18.54" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{FC38DB41-2593-4AE3-890A-83FAE8D7361F}">
-    <text>many small inaccuracies</text>
-  </threadedComment>
   <threadedComment ref="D20" dT="2021-05-07T20:37:27.60" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{CABCC935-D353-49C6-BF7B-26945C3B7EEC}">
     <text>no dragdrop</text>
   </threadedComment>
   <threadedComment ref="D32" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}">
     <text>require toolbar's combobox and dropdownbtn</text>
   </threadedComment>
-  <threadedComment ref="D38" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{2E4E5FAA-8920-4E1C-B04E-22732D846631}">
-    <text>other inaccuracies</text>
-  </threadedComment>
   <threadedComment ref="D51" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{2E4E5FAA-8920-4E1D-B04E-22732D846631}">
     <text>first image not fitted to window</text>
   </threadedComment>
   <threadedComment ref="D54" dT="2021-05-08T19:23:42.84" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{08B0E8B2-B025-4593-86AB-65151186337D}">
     <text>no charts</text>
-  </threadedComment>
-  <threadedComment ref="D66" dT="2021-05-08T19:23:42.84" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{D1AD9B46-69A2-4F80-ADD4-0B51A5891E85}">
-    <text>not works lists</text>
   </threadedComment>
   <threadedComment ref="D68" dT="2021-05-07T19:42:23.30" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{BD118A23-46B1-45EB-A479-612E3372B34F}">
     <text>lines without arrow's caps</text>
@@ -2319,48 +2185,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="14"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="F1" s="37"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="37"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2368,22 +2228,16 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2392,32 +2246,28 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -2426,14 +2276,12 @@
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2442,14 +2290,12 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -2457,15 +2303,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="10" t="s">
-        <v>97</v>
+      <c r="D7" s="41" t="s">
+        <v>96</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -2474,14 +2318,12 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -2490,14 +2332,12 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2506,14 +2346,12 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -2522,14 +2360,12 @@
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -2538,14 +2374,12 @@
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -2554,14 +2388,12 @@
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2570,14 +2402,12 @@
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -2586,14 +2416,12 @@
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -2602,14 +2430,12 @@
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -2618,14 +2444,12 @@
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -2634,14 +2458,12 @@
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2650,14 +2472,12 @@
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -2666,14 +2486,12 @@
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -2682,14 +2500,12 @@
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -2698,14 +2514,12 @@
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
@@ -2714,14 +2528,12 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -2730,14 +2542,12 @@
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
@@ -2746,14 +2556,12 @@
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -2761,15 +2569,13 @@
         <v>27</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="12" t="s">
-        <v>97</v>
+      <c r="D26" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
@@ -2777,15 +2583,13 @@
         <v>28</v>
       </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="12" t="s">
-        <v>97</v>
+      <c r="D27" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -2794,14 +2598,12 @@
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
@@ -2810,14 +2612,12 @@
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
@@ -2826,14 +2626,12 @@
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
@@ -2842,14 +2640,12 @@
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
@@ -2858,14 +2654,12 @@
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
@@ -2874,14 +2668,12 @@
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
@@ -2890,14 +2682,12 @@
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>2</v>
       </c>
@@ -2906,14 +2696,12 @@
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
@@ -2922,14 +2710,12 @@
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
@@ -2938,14 +2724,12 @@
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>2</v>
       </c>
@@ -2954,14 +2738,12 @@
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
@@ -2970,14 +2752,12 @@
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
@@ -2986,14 +2766,12 @@
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>2</v>
       </c>
@@ -3002,14 +2780,12 @@
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
@@ -3018,14 +2794,12 @@
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -3034,14 +2808,12 @@
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
@@ -3050,14 +2822,12 @@
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>2</v>
       </c>
@@ -3066,14 +2836,12 @@
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>2</v>
       </c>
@@ -3082,14 +2850,12 @@
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>2</v>
       </c>
@@ -3098,14 +2864,12 @@
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>2</v>
       </c>
@@ -3114,14 +2878,12 @@
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>2</v>
       </c>
@@ -3130,14 +2892,12 @@
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>2</v>
       </c>
@@ -3146,14 +2906,12 @@
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
@@ -3162,14 +2920,12 @@
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
@@ -3178,14 +2934,12 @@
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
@@ -3194,14 +2948,12 @@
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>2</v>
       </c>
@@ -3210,14 +2962,12 @@
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>2</v>
       </c>
@@ -3226,14 +2976,12 @@
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>2</v>
       </c>
@@ -3242,14 +2990,12 @@
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
@@ -3258,14 +3004,12 @@
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>2</v>
       </c>
@@ -3274,14 +3018,12 @@
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>2</v>
       </c>
@@ -3290,14 +3032,12 @@
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
@@ -3306,14 +3046,12 @@
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>2</v>
       </c>
@@ -3322,14 +3060,12 @@
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>2</v>
       </c>
@@ -3338,14 +3074,12 @@
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>2</v>
       </c>
@@ -3354,14 +3088,12 @@
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>2</v>
       </c>
@@ -3370,14 +3102,12 @@
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>2</v>
       </c>
@@ -3386,14 +3116,12 @@
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>2</v>
       </c>
@@ -3402,14 +3130,12 @@
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E66" s="4"/>
       <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
@@ -3418,14 +3144,12 @@
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E67" s="4"/>
       <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>3</v>
       </c>
@@ -3434,14 +3158,12 @@
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E68" s="4"/>
       <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>3</v>
       </c>
@@ -3450,14 +3172,12 @@
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>3</v>
       </c>
@@ -3466,14 +3186,12 @@
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E70" s="4"/>
       <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>3</v>
       </c>
@@ -3482,14 +3200,12 @@
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>3</v>
       </c>
@@ -3498,14 +3214,12 @@
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>3</v>
       </c>
@@ -3514,14 +3228,12 @@
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E73" s="4"/>
       <c r="F73" s="4"/>
-      <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>3</v>
       </c>
@@ -3530,50 +3242,42 @@
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
-      <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C75" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D75" s="9" t="s">
-        <v>100</v>
+      <c r="C75" s="5"/>
+      <c r="D75" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
-      <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>3</v>
       </c>
@@ -3582,14 +3286,12 @@
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
-      <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>3</v>
       </c>
@@ -3598,14 +3300,12 @@
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>3</v>
       </c>
@@ -3614,14 +3314,12 @@
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>3</v>
       </c>
@@ -3630,14 +3328,12 @@
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
-      <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>3</v>
       </c>
@@ -3646,14 +3342,12 @@
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
@@ -3662,14 +3356,12 @@
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
@@ -3678,14 +3370,12 @@
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E83" s="4"/>
       <c r="F83" s="4"/>
-      <c r="G83" s="4"/>
-      <c r="H83" s="4"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
@@ -3694,14 +3384,12 @@
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E84" s="4"/>
       <c r="F84" s="4"/>
-      <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
@@ -3710,32 +3398,28 @@
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B86" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C86" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C86" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="D86" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>3</v>
       </c>
@@ -3744,14 +3428,12 @@
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E87" s="4"/>
       <c r="F87" s="4"/>
-      <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>3</v>
       </c>
@@ -3760,104 +3442,92 @@
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E88" s="4"/>
       <c r="F88" s="4"/>
-      <c r="G88" s="4"/>
-      <c r="H88" s="4"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E89" s="4"/>
       <c r="F89" s="4"/>
-      <c r="G89" s="4"/>
-      <c r="H89" s="4"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E90" s="4"/>
       <c r="F90" s="4"/>
-      <c r="G90" s="4"/>
-      <c r="H90" s="4"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D91" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E91" s="4"/>
       <c r="F91" s="4"/>
-      <c r="G91" s="4"/>
-      <c r="H91" s="4"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
-      <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E93" s="4"/>
       <c r="F93" s="4"/>
-      <c r="G93" s="4"/>
-      <c r="H93" s="4"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>3</v>
       </c>
@@ -3866,14 +3536,12 @@
       </c>
       <c r="C94" s="5"/>
       <c r="D94" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E94" s="4"/>
       <c r="F94" s="4"/>
-      <c r="G94" s="4"/>
-      <c r="H94" s="4"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>3</v>
       </c>
@@ -3882,14 +3550,12 @@
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
-      <c r="G95" s="4"/>
-      <c r="H95" s="4"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>3</v>
       </c>
@@ -3898,42 +3564,35 @@
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E96" s="4"/>
       <c r="F96" s="4"/>
-      <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="7"/>
       <c r="B97" s="7">
         <f>COUNTA(B3:B96)</f>
         <v>94</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D97" s="8">
         <f>COUNTIF(D3:D96,"identic")/$B$97</f>
-        <v>0.87234042553191493</v>
+        <v>0.88297872340425532</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="8">
         <f>COUNTIF(F3:F96,"identic")/$B$97</f>
         <v>0</v>
       </c>
-      <c r="G97" s="7"/>
-      <c r="H97" s="8">
-        <f>COUNTIF(H3:H96,"identic")/$B$97</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D98" s="8">
         <f>COUNTA(D3:D96)/$B$97</f>
@@ -3944,29 +3603,23 @@
         <f>COUNTA(F3:F96)/$B$97</f>
         <v>0</v>
       </c>
-      <c r="G98" s="7"/>
-      <c r="H98" s="8">
-        <f>COUNTA(H3:H96)/$B$97</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>99</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:H96"/>
-  <mergeCells count="4">
+  <autoFilter ref="A2:F96" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3975,1044 +3628,1044 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="16"/>
-    <col min="2" max="2" width="62" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="62.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="9.109375" style="14"/>
+    <col min="2" max="2" width="62" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="62.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="38"/>
+      <c r="E1" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="15" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="38"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="E2" s="15"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="C4" s="22">
+        <v>1</v>
+      </c>
+      <c r="D4" s="22">
+        <v>1</v>
+      </c>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="24">
-        <v>1</v>
-      </c>
-      <c r="D4" s="24">
-        <v>1</v>
-      </c>
-      <c r="E4" s="25"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="C5" s="22">
+        <v>1</v>
+      </c>
+      <c r="D5" s="24">
+        <v>0</v>
+      </c>
+      <c r="E5" s="25"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="24">
-        <v>1</v>
-      </c>
-      <c r="D5" s="26">
+      <c r="B6" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22">
+        <v>1</v>
+      </c>
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="22">
+        <v>1</v>
+      </c>
+      <c r="D7" s="22">
+        <v>1</v>
+      </c>
+      <c r="E7" s="25"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
+      <c r="D8" s="22">
+        <v>1</v>
+      </c>
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="22">
+        <v>1</v>
+      </c>
+      <c r="D9" s="22">
+        <v>1</v>
+      </c>
+      <c r="E9" s="26"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="22">
+        <v>1</v>
+      </c>
+      <c r="D10" s="22">
+        <v>1</v>
+      </c>
+      <c r="E10" s="26"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C11" s="22">
+        <v>1</v>
+      </c>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="26"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="22">
+        <v>1</v>
+      </c>
+      <c r="D12" s="22">
+        <v>1</v>
+      </c>
+      <c r="E12" s="26"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" s="22">
+        <v>1</v>
+      </c>
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
+      <c r="E13" s="26"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="22">
+        <v>1</v>
+      </c>
+      <c r="D14" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="E14" s="26"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
+      <c r="D15" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="E15" s="26"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="22">
+        <v>1</v>
+      </c>
+      <c r="D16" s="22">
+        <v>1</v>
+      </c>
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" s="22">
+        <v>1</v>
+      </c>
+      <c r="D17" s="24">
         <v>0</v>
       </c>
-      <c r="E5" s="27"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="24">
-        <v>1</v>
-      </c>
-      <c r="D6" s="24">
-        <v>1</v>
-      </c>
-      <c r="E6" s="27"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="24">
-        <v>1</v>
-      </c>
-      <c r="D7" s="24">
-        <v>1</v>
-      </c>
-      <c r="E7" s="27"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="24">
-        <v>1</v>
-      </c>
-      <c r="D8" s="24">
-        <v>1</v>
-      </c>
-      <c r="E8" s="28"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="24">
-        <v>1</v>
-      </c>
-      <c r="D9" s="24">
-        <v>1</v>
-      </c>
-      <c r="E9" s="28"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="C10" s="24">
-        <v>1</v>
-      </c>
-      <c r="D10" s="24">
-        <v>1</v>
-      </c>
-      <c r="E10" s="28"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C11" s="24">
-        <v>1</v>
-      </c>
-      <c r="D11" s="24">
-        <v>1</v>
-      </c>
-      <c r="E11" s="28"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C12" s="24">
-        <v>1</v>
-      </c>
-      <c r="D12" s="24">
-        <v>1</v>
-      </c>
-      <c r="E12" s="28"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="C13" s="24">
-        <v>1</v>
-      </c>
-      <c r="D13" s="24">
-        <v>1</v>
-      </c>
-      <c r="E13" s="28"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="C14" s="24">
-        <v>1</v>
-      </c>
-      <c r="D14" s="29">
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C18" s="22">
+        <v>1</v>
+      </c>
+      <c r="D18" s="24">
+        <v>0</v>
+      </c>
+      <c r="E18" s="26"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" s="22">
+        <v>1</v>
+      </c>
+      <c r="D19" s="22">
+        <v>1</v>
+      </c>
+      <c r="E19" s="26"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C20" s="22">
+        <v>1</v>
+      </c>
+      <c r="D20" s="28">
+        <v>0</v>
+      </c>
+      <c r="E20" s="26"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="22">
+        <v>1</v>
+      </c>
+      <c r="D21" s="22">
+        <v>1</v>
+      </c>
+      <c r="E21" s="26"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C22" s="22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="26"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="22">
+        <v>1</v>
+      </c>
+      <c r="D23" s="22">
+        <v>1</v>
+      </c>
+      <c r="E23" s="26"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="22">
+        <v>1</v>
+      </c>
+      <c r="D24" s="22">
+        <v>1</v>
+      </c>
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" s="22">
+        <v>1</v>
+      </c>
+      <c r="D25" s="22">
+        <v>1</v>
+      </c>
+      <c r="E25" s="26"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="24">
+        <v>0</v>
+      </c>
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="22">
+        <v>1</v>
+      </c>
+      <c r="E27" s="26"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C28" s="22">
+        <v>1</v>
+      </c>
+      <c r="D28" s="22">
+        <v>1</v>
+      </c>
+      <c r="E28" s="26"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C29" s="22">
+        <v>1</v>
+      </c>
+      <c r="D29" s="28">
+        <v>0</v>
+      </c>
+      <c r="E29" s="26"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" s="22">
+        <v>1</v>
+      </c>
+      <c r="D30" s="22">
+        <v>1</v>
+      </c>
+      <c r="E30" s="26"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" s="22">
+        <v>1</v>
+      </c>
+      <c r="D31" s="22">
+        <v>1</v>
+      </c>
+      <c r="E31" s="26"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" s="22">
+        <v>1</v>
+      </c>
+      <c r="D32" s="22">
+        <v>1</v>
+      </c>
+      <c r="E32" s="26"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C33" s="22">
+        <v>1</v>
+      </c>
+      <c r="D33" s="22">
+        <v>1</v>
+      </c>
+      <c r="E33" s="26"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" s="22">
+        <v>1</v>
+      </c>
+      <c r="D34" s="22">
+        <v>1</v>
+      </c>
+      <c r="E34" s="26"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="40"/>
+      <c r="E35" s="26"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="22">
+        <v>1</v>
+      </c>
+      <c r="D36" s="22">
+        <v>1</v>
+      </c>
+      <c r="E36" s="26"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C37" s="22">
+        <v>1</v>
+      </c>
+      <c r="D37" s="28">
+        <v>0</v>
+      </c>
+      <c r="E37" s="26"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C38" s="22">
+        <v>1</v>
+      </c>
+      <c r="D38" s="22">
+        <v>1</v>
+      </c>
+      <c r="E38" s="26"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C39" s="22">
+        <v>1</v>
+      </c>
+      <c r="D39" s="28">
+        <v>0</v>
+      </c>
+      <c r="E39" s="26"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" s="22">
+        <v>1</v>
+      </c>
+      <c r="D40" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="E40" s="26"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C41" s="22">
+        <v>1</v>
+      </c>
+      <c r="D41" s="22">
+        <v>1</v>
+      </c>
+      <c r="E41" s="26"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C42" s="22">
+        <v>1</v>
+      </c>
+      <c r="D42" s="22">
+        <v>1</v>
+      </c>
+      <c r="E42" s="26"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" s="22">
+        <v>1</v>
+      </c>
+      <c r="D43" s="28">
+        <v>0</v>
+      </c>
+      <c r="E43" s="26"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="20"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="26"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="19"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" s="22">
+        <v>1</v>
+      </c>
+      <c r="D46" s="22">
+        <v>1</v>
+      </c>
+      <c r="E46" s="26"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="C47" s="22">
+        <v>1</v>
+      </c>
+      <c r="D47" s="22">
+        <v>1</v>
+      </c>
+      <c r="E47" s="26"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" s="22">
+        <v>1</v>
+      </c>
+      <c r="D48" s="22">
+        <v>1</v>
+      </c>
+      <c r="E48" s="26"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="C49" s="22">
+        <v>1</v>
+      </c>
+      <c r="D49" s="22">
+        <v>1</v>
+      </c>
+      <c r="E49" s="26"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C50" s="22">
+        <v>1</v>
+      </c>
+      <c r="D50" s="22">
+        <v>1</v>
+      </c>
+      <c r="E50" s="26"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C51" s="22">
+        <v>1</v>
+      </c>
+      <c r="D51" s="22">
+        <v>1</v>
+      </c>
+      <c r="E51" s="26"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C52" s="22">
+        <v>1</v>
+      </c>
+      <c r="D52" s="22">
+        <v>1</v>
+      </c>
+      <c r="E52" s="26"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C53" s="22">
+        <v>1</v>
+      </c>
+      <c r="D53" s="22">
+        <v>1</v>
+      </c>
+      <c r="E53" s="26"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C54" s="27">
         <v>0.75</v>
       </c>
-      <c r="E14" s="28"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" s="24">
-        <v>1</v>
-      </c>
-      <c r="D15" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="28"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="24">
-        <v>1</v>
-      </c>
-      <c r="D16" s="24">
-        <v>1</v>
-      </c>
-      <c r="E16" s="28"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="C17" s="24">
-        <v>1</v>
-      </c>
-      <c r="D17" s="26">
+      <c r="D54" s="22">
+        <v>1</v>
+      </c>
+      <c r="E54" s="26" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="C55" s="22">
+        <v>1</v>
+      </c>
+      <c r="D55" s="22">
+        <v>1</v>
+      </c>
+      <c r="E55" s="26"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="B56" s="26"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="26"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="19"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C58" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="D58" s="28">
         <v>0</v>
       </c>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="C18" s="24">
-        <v>1</v>
-      </c>
-      <c r="D18" s="26">
+      <c r="E58" s="26" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="20" t="s">
+        <v>234</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="C59" s="22">
+        <v>1</v>
+      </c>
+      <c r="D59" s="24">
         <v>0</v>
       </c>
-      <c r="E18" s="28"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" s="24">
-        <v>1</v>
-      </c>
-      <c r="D19" s="24">
-        <v>1</v>
-      </c>
-      <c r="E19" s="28"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" s="24">
-        <v>1</v>
-      </c>
-      <c r="D20" s="30">
+      <c r="E59" s="26"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="C60" s="22">
+        <v>1</v>
+      </c>
+      <c r="D60" s="24">
         <v>0</v>
       </c>
-      <c r="E20" s="28"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="C21" s="24">
-        <v>1</v>
-      </c>
-      <c r="D21" s="24">
-        <v>1</v>
-      </c>
-      <c r="E21" s="28"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="C22" s="24">
-        <v>1</v>
-      </c>
-      <c r="D22" s="24">
-        <v>1</v>
-      </c>
-      <c r="E22" s="28"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" s="24">
-        <v>1</v>
-      </c>
-      <c r="D23" s="24">
-        <v>1</v>
-      </c>
-      <c r="E23" s="28"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="C24" s="24">
-        <v>1</v>
-      </c>
-      <c r="D24" s="24">
-        <v>1</v>
-      </c>
-      <c r="E24" s="28"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="C25" s="24">
-        <v>1</v>
-      </c>
-      <c r="D25" s="24">
-        <v>1</v>
-      </c>
-      <c r="E25" s="28"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>170</v>
-      </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="26">
+      <c r="E60" s="26"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C61" s="22">
+        <v>1</v>
+      </c>
+      <c r="D61" s="24">
         <v>0</v>
       </c>
-      <c r="E26" s="28"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="26">
+      <c r="E61" s="26"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C62" s="22">
+        <v>1</v>
+      </c>
+      <c r="D62" s="24">
         <v>0</v>
       </c>
-      <c r="E27" s="28"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>174</v>
-      </c>
-      <c r="C28" s="24">
-        <v>1</v>
-      </c>
-      <c r="D28" s="24">
-        <v>1</v>
-      </c>
-      <c r="E28" s="28"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="B29" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="C29" s="24">
-        <v>1</v>
-      </c>
-      <c r="D29" s="30">
+      <c r="E62" s="26"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="C63" s="22">
+        <v>1</v>
+      </c>
+      <c r="D63" s="24">
         <v>0</v>
       </c>
-      <c r="E29" s="28"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="C30" s="24">
-        <v>1</v>
-      </c>
-      <c r="D30" s="24">
-        <v>1</v>
-      </c>
-      <c r="E30" s="28"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="C31" s="24">
-        <v>1</v>
-      </c>
-      <c r="D31" s="24">
-        <v>1</v>
-      </c>
-      <c r="E31" s="28"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="C32" s="24">
-        <v>1</v>
-      </c>
-      <c r="D32" s="24">
-        <v>1</v>
-      </c>
-      <c r="E32" s="28"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>184</v>
-      </c>
-      <c r="C33" s="24">
-        <v>1</v>
-      </c>
-      <c r="D33" s="24">
-        <v>1</v>
-      </c>
-      <c r="E33" s="28"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="C34" s="24">
-        <v>1</v>
-      </c>
-      <c r="D34" s="24">
-        <v>1</v>
-      </c>
-      <c r="E34" s="28"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="C35" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="D35" s="33"/>
-      <c r="E35" s="28"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="C36" s="24">
-        <v>1</v>
-      </c>
-      <c r="D36" s="24">
-        <v>1</v>
-      </c>
-      <c r="E36" s="28"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="B37" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C37" s="24">
-        <v>1</v>
-      </c>
-      <c r="D37" s="30">
+      <c r="E63" s="26"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="C64" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="D64" s="24">
         <v>0</v>
       </c>
-      <c r="E37" s="28"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="B38" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="C38" s="24">
-        <v>1</v>
-      </c>
-      <c r="D38" s="24">
-        <v>1</v>
-      </c>
-      <c r="E38" s="28"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="B39" s="23" t="s">
-        <v>197</v>
-      </c>
-      <c r="C39" s="24">
-        <v>1</v>
-      </c>
-      <c r="D39" s="30">
+      <c r="E64" s="26" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="C65" s="22">
+        <v>1</v>
+      </c>
+      <c r="D65" s="24">
         <v>0</v>
       </c>
-      <c r="E39" s="28"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="B40" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="C40" s="24">
-        <v>1</v>
-      </c>
-      <c r="D40" s="29">
-        <v>0.5</v>
-      </c>
-      <c r="E40" s="28"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="B41" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="C41" s="24">
-        <v>1</v>
-      </c>
-      <c r="D41" s="29">
-        <v>0.9</v>
-      </c>
-      <c r="E41" s="28"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="B42" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="C42" s="24">
-        <v>1</v>
-      </c>
-      <c r="D42" s="24">
-        <v>1</v>
-      </c>
-      <c r="E42" s="28"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="C43" s="24">
-        <v>1</v>
-      </c>
-      <c r="D43" s="30">
+      <c r="E65" s="26"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="26" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="C67" s="22">
+        <v>1</v>
+      </c>
+      <c r="D67" s="24">
         <v>0</v>
       </c>
-      <c r="E43" s="28"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="28"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="21"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="B46" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="C46" s="24">
-        <v>1</v>
-      </c>
-      <c r="D46" s="24">
-        <v>1</v>
-      </c>
-      <c r="E46" s="28"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="B47" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="C47" s="24">
-        <v>1</v>
-      </c>
-      <c r="D47" s="24">
-        <v>1</v>
-      </c>
-      <c r="E47" s="28"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="B48" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="C48" s="24">
-        <v>1</v>
-      </c>
-      <c r="D48" s="24">
-        <v>1</v>
-      </c>
-      <c r="E48" s="28"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="B49" s="23" t="s">
-        <v>215</v>
-      </c>
-      <c r="C49" s="24">
-        <v>1</v>
-      </c>
-      <c r="D49" s="24">
-        <v>1</v>
-      </c>
-      <c r="E49" s="28"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="B50" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="C50" s="24">
-        <v>1</v>
-      </c>
-      <c r="D50" s="24">
-        <v>1</v>
-      </c>
-      <c r="E50" s="28"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B51" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="C51" s="24">
-        <v>1</v>
-      </c>
-      <c r="D51" s="24">
-        <v>1</v>
-      </c>
-      <c r="E51" s="28"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="B52" s="23" t="s">
-        <v>221</v>
-      </c>
-      <c r="C52" s="24">
-        <v>1</v>
-      </c>
-      <c r="D52" s="24">
-        <v>1</v>
-      </c>
-      <c r="E52" s="28"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>223</v>
-      </c>
-      <c r="C53" s="24">
-        <v>1</v>
-      </c>
-      <c r="D53" s="24">
-        <v>1</v>
-      </c>
-      <c r="E53" s="28"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="B54" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="C54" s="29">
-        <v>0.75</v>
-      </c>
-      <c r="D54" s="24">
-        <v>1</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="B55" s="23" t="s">
-        <v>228</v>
-      </c>
-      <c r="C55" s="24">
-        <v>1</v>
-      </c>
-      <c r="D55" s="24">
-        <v>1</v>
-      </c>
-      <c r="E55" s="28"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="35" t="s">
-        <v>229</v>
-      </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="28"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="21"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="B58" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="C58" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="D58" s="30">
+      <c r="E67" s="26"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="26" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="31" t="s">
+        <v>257</v>
+      </c>
+      <c r="B69" s="26"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="26"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="16" t="s">
+        <v>258</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="C70" s="22">
+        <v>1</v>
+      </c>
+      <c r="D70" s="24">
         <v>0</v>
       </c>
-      <c r="E58" s="28" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
-        <v>235</v>
-      </c>
-      <c r="B59" s="23" t="s">
-        <v>236</v>
-      </c>
-      <c r="C59" s="24">
-        <v>1</v>
-      </c>
-      <c r="D59" s="26">
-        <v>0</v>
-      </c>
-      <c r="E59" s="28"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
-        <v>237</v>
-      </c>
-      <c r="B60" s="23" t="s">
-        <v>238</v>
-      </c>
-      <c r="C60" s="24">
-        <v>1</v>
-      </c>
-      <c r="D60" s="26">
-        <v>0</v>
-      </c>
-      <c r="E60" s="28"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="B61" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="C61" s="24">
-        <v>1</v>
-      </c>
-      <c r="D61" s="26">
-        <v>0</v>
-      </c>
-      <c r="E61" s="28"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="B62" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="C62" s="24">
-        <v>1</v>
-      </c>
-      <c r="D62" s="26">
-        <v>0</v>
-      </c>
-      <c r="E62" s="28"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
-        <v>243</v>
-      </c>
-      <c r="B63" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="C63" s="24">
-        <v>1</v>
-      </c>
-      <c r="D63" s="26">
-        <v>0</v>
-      </c>
-      <c r="E63" s="28"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="B64" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="C64" s="29">
-        <v>0.75</v>
-      </c>
-      <c r="D64" s="26">
-        <v>0</v>
-      </c>
-      <c r="E64" s="28" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="B65" s="23" t="s">
-        <v>249</v>
-      </c>
-      <c r="C65" s="24">
-        <v>1</v>
-      </c>
-      <c r="D65" s="26">
-        <v>0</v>
-      </c>
-      <c r="E65" s="28"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="B66" s="23" t="s">
-        <v>251</v>
-      </c>
-      <c r="C66" s="31"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="28" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>254</v>
-      </c>
-      <c r="C67" s="24">
-        <v>1</v>
-      </c>
-      <c r="D67" s="26">
-        <v>0</v>
-      </c>
-      <c r="E67" s="28"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="B68" s="23" t="s">
-        <v>256</v>
-      </c>
-      <c r="C68" s="31"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="28" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="35" t="s">
-        <v>258</v>
-      </c>
-      <c r="B69" s="28"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="28"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="B70" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="C70" s="24">
-        <v>1</v>
-      </c>
-      <c r="D70" s="26">
-        <v>0</v>
-      </c>
-      <c r="E70" s="21"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="38"/>
-      <c r="B71" s="39"/>
-      <c r="C71" s="40">
+      <c r="E70" s="19"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="34"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="36">
         <f>AVERAGE(C3:C70)</f>
         <v>0.98947368421052628</v>
       </c>
-      <c r="D71" s="40">
+      <c r="D71" s="36">
         <f>AVERAGE(D3:D70)</f>
-        <v>0.63813559322033897</v>
-      </c>
-      <c r="E71" s="39"/>
+        <v>0.65677966101694918</v>
+      </c>
+      <c r="E71" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
GKv2/GKv3 compatibility fixes (2), printing restore
</commit_message>
<xml_diff>
--- a/dev_info/gk_compatibility_matrix.xlsx
+++ b/dev_info/gk_compatibility_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKS\shared\gkdev\GEDKeeper\dev_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB49238-4385-467E-B10C-B565134B60E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F71248C-F61D-4B81-A8E2-8826DFFE6775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compatibility Matrix" sheetId="2" r:id="rId1"/>
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="262">
   <si>
     <t>Module</t>
   </si>
@@ -1048,6 +1048,12 @@
   <si>
     <t>Distribution for Linux (Debian/Ubuntu)</t>
   </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>Printing charts (circle, tree)</t>
+  </si>
 </sst>
 </file>
 
@@ -1056,7 +1062,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1245,6 +1251,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="43">
@@ -1772,6 +1785,9 @@
     <xf numFmtId="10" fontId="16" fillId="35" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="42" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1783,9 +1799,6 @@
     </xf>
     <xf numFmtId="2" fontId="16" fillId="41" borderId="12" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="42" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -2188,9 +2201,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2204,23 +2217,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37" t="s">
+      <c r="D1" s="38"/>
+      <c r="E1" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="37"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
+      <c r="A2" s="38"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2289,7 +2302,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="37" t="s">
         <v>96</v>
       </c>
       <c r="E6" s="4"/>
@@ -2303,7 +2316,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="37" t="s">
         <v>96</v>
       </c>
       <c r="E7" s="4"/>
@@ -2345,7 +2358,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="37" t="s">
         <v>96</v>
       </c>
       <c r="E10" s="4"/>
@@ -2485,7 +2498,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="37" t="s">
         <v>96</v>
       </c>
       <c r="E20" s="4"/>
@@ -2779,8 +2792,8 @@
         <v>42</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="9" t="s">
-        <v>99</v>
+      <c r="D41" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -3580,7 +3593,7 @@
       </c>
       <c r="D97" s="8">
         <f>COUNTIF(D3:D96,"identic")/$B$97</f>
-        <v>0.88297872340425532</v>
+        <v>0.8936170212765957</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="8">
@@ -3629,10 +3642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3645,30 +3658,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="39" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="15" t="s">
         <v>120</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
@@ -3886,8 +3899,8 @@
       <c r="C17" s="22">
         <v>1</v>
       </c>
-      <c r="D17" s="24">
-        <v>0</v>
+      <c r="D17" s="22">
+        <v>1</v>
       </c>
       <c r="E17" s="26"/>
     </row>
@@ -4149,10 +4162,10 @@
       <c r="B35" s="21" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="39" t="s">
+      <c r="C35" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="D35" s="40"/>
+      <c r="D35" s="41"/>
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -4276,44 +4289,42 @@
       <c r="E43" s="26"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="20"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30"/>
+      <c r="A44" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="22">
+        <v>1</v>
+      </c>
       <c r="E44" s="26"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="20"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="26"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B46" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="19"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="C46" s="22">
-        <v>1</v>
-      </c>
-      <c r="D46" s="22">
-        <v>1</v>
-      </c>
-      <c r="E46" s="26"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="19"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C47" s="22">
         <v>1</v>
@@ -4325,10 +4336,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C48" s="22">
         <v>1</v>
@@ -4340,10 +4351,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C49" s="22">
         <v>1</v>
@@ -4355,10 +4366,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C50" s="22">
         <v>1</v>
@@ -4370,10 +4381,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C51" s="22">
         <v>1</v>
@@ -4385,10 +4396,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C52" s="22">
         <v>1</v>
@@ -4400,10 +4411,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C53" s="22">
         <v>1</v>
@@ -4415,94 +4426,94 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="C54" s="27">
-        <v>0.75</v>
+        <v>222</v>
+      </c>
+      <c r="C54" s="22">
+        <v>1</v>
       </c>
       <c r="D54" s="22">
         <v>1</v>
       </c>
-      <c r="E54" s="26" t="s">
-        <v>225</v>
-      </c>
+      <c r="E54" s="26"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C55" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="D55" s="22">
+        <v>1</v>
+      </c>
+      <c r="E55" s="26" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="20" t="s">
         <v>226</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B56" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="C55" s="22">
-        <v>1</v>
-      </c>
-      <c r="D55" s="22">
-        <v>1</v>
-      </c>
-      <c r="E55" s="26"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="31" t="s">
+      <c r="C56" s="22">
+        <v>1</v>
+      </c>
+      <c r="D56" s="22">
+        <v>1</v>
+      </c>
+      <c r="E56" s="26"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="30"/>
-      <c r="E56" s="26"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="16" t="s">
+      <c r="B57" s="26"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="30"/>
+      <c r="E57" s="26"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B58" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="19"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="B58" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="C58" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="D58" s="28">
-        <v>0</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>233</v>
-      </c>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="19"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B59" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="C59" s="22">
-        <v>1</v>
-      </c>
-      <c r="D59" s="24">
+        <v>232</v>
+      </c>
+      <c r="C59" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="D59" s="28">
         <v>0</v>
       </c>
-      <c r="E59" s="26"/>
+      <c r="E59" s="26" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C60" s="22">
         <v>1</v>
@@ -4514,10 +4525,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C61" s="22">
         <v>1</v>
@@ -4529,10 +4540,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C62" s="22">
         <v>1</v>
@@ -4544,10 +4555,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C63" s="22">
         <v>1</v>
@@ -4559,113 +4570,128 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>245</v>
-      </c>
-      <c r="C64" s="27">
-        <v>0.75</v>
+        <v>243</v>
+      </c>
+      <c r="C64" s="22">
+        <v>1</v>
       </c>
       <c r="D64" s="24">
         <v>0</v>
       </c>
-      <c r="E64" s="26" t="s">
-        <v>246</v>
-      </c>
+      <c r="E64" s="26"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="C65" s="22">
-        <v>1</v>
+        <v>245</v>
+      </c>
+      <c r="C65" s="27">
+        <v>0.75</v>
       </c>
       <c r="D65" s="24">
         <v>0</v>
       </c>
-      <c r="E65" s="26"/>
+      <c r="E65" s="26" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="C66" s="29"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="26" t="s">
-        <v>251</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="C66" s="22">
+        <v>1</v>
+      </c>
+      <c r="D66" s="24">
+        <v>0</v>
+      </c>
+      <c r="E66" s="26"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="C67" s="22">
-        <v>1</v>
-      </c>
-      <c r="D67" s="24">
-        <v>0</v>
-      </c>
-      <c r="E67" s="26"/>
+        <v>250</v>
+      </c>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="26" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="C68" s="22">
+        <v>1</v>
+      </c>
+      <c r="D68" s="24">
+        <v>0</v>
+      </c>
+      <c r="E68" s="26"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="B68" s="21" t="s">
+      <c r="B69" s="21" t="s">
         <v>255</v>
       </c>
-      <c r="C68" s="29"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="26" t="s">
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="26" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="31" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="B69" s="26"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="33"/>
-      <c r="E69" s="26"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="16" t="s">
+      <c r="B70" s="26"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="26"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B71" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="C70" s="22">
-        <v>1</v>
-      </c>
-      <c r="D70" s="24">
+      <c r="C71" s="22">
+        <v>1</v>
+      </c>
+      <c r="D71" s="24">
         <v>0</v>
       </c>
-      <c r="E70" s="19"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="34"/>
-      <c r="B71" s="35"/>
-      <c r="C71" s="36">
-        <f>AVERAGE(C3:C70)</f>
+      <c r="E71" s="19"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="34"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="36">
+        <f>AVERAGE(C3:C71)</f>
         <v>0.98947368421052628</v>
       </c>
-      <c r="D71" s="36">
-        <f>AVERAGE(D3:D70)</f>
-        <v>0.65677966101694918</v>
-      </c>
-      <c r="E71" s="35"/>
+      <c r="D72" s="36">
+        <f>AVERAGE(D3:D71)</f>
+        <v>0.6791666666666667</v>
+      </c>
+      <c r="E72" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4675,6 +4701,7 @@
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="C35:D35"/>
   </mergeCells>
+  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
GKv3: restoring charts in statistics
</commit_message>
<xml_diff>
--- a/dev_info/gk_compatibility_matrix.xlsx
+++ b/dev_info/gk_compatibility_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKS\shared\gkdev\GEDKeeper\dev_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F71248C-F61D-4B81-A8E2-8826DFFE6775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290D95D4-D891-4D15-96A4-370E17A0EEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,6 @@
     <author>tc={CABCC935-D353-49C6-BF7B-26945C3B7EEC}</author>
     <author>tc={4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}</author>
     <author>tc={2E4E5FAA-8920-4E1D-B04E-22732D846631}</author>
-    <author>tc={08B0E8B2-B025-4593-86AB-65151186337D}</author>
     <author>tc={BD118A23-46B1-45EB-A479-612E3372B34F}</author>
     <author>tc={34F4FF22-A13C-482B-B521-D1FCFDCF8C10}</author>
     <author>tc={D1AD9B46-69A2-4F81-ADD4-0B51A5891E85}</author>
@@ -98,15 +97,7 @@
     first image not fitted to window</t>
       </text>
     </comment>
-    <comment ref="D54" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
-      <text>
-        <t>[Цепочка примечаний]
-Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
-Комментарий:
-    no charts</t>
-      </text>
-    </comment>
-    <comment ref="D68" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="D68" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <t>[Цепочка примечаний]
 Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
@@ -114,7 +105,7 @@
     lines without arrow's caps</t>
       </text>
     </comment>
-    <comment ref="D74" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="D74" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <t>[Цепочка примечаний]
 Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
@@ -122,7 +113,7 @@
     many errors and dont work sorting</t>
       </text>
     </comment>
-    <comment ref="D77" authorId="9" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="D77" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <t>[Цепочка примечаний]
 Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
@@ -192,7 +183,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -223,7 +214,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="264">
   <si>
     <t>Module</t>
   </si>
@@ -791,9 +782,6 @@
     <t>Statistics</t>
   </si>
   <si>
-    <t>1.21.1</t>
-  </si>
-  <si>
     <t>Charts (line, bars)</t>
   </si>
   <si>
@@ -1053,6 +1041,15 @@
   </si>
   <si>
     <t>Printing charts (circle, tree)</t>
+  </si>
+  <si>
+    <t>1.12.1</t>
+  </si>
+  <si>
+    <t>Specific person filtration</t>
+  </si>
+  <si>
+    <t>1.20.1</t>
   </si>
 </sst>
 </file>
@@ -2182,9 +2179,6 @@
   <threadedComment ref="D51" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{2E4E5FAA-8920-4E1D-B04E-22732D846631}">
     <text>first image not fitted to window</text>
   </threadedComment>
-  <threadedComment ref="D54" dT="2021-05-08T19:23:42.84" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{08B0E8B2-B025-4593-86AB-65151186337D}">
-    <text>no charts</text>
-  </threadedComment>
   <threadedComment ref="D68" dT="2021-05-07T19:42:23.30" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{BD118A23-46B1-45EB-A479-612E3372B34F}">
     <text>lines without arrow's caps</text>
   </threadedComment>
@@ -2203,7 +2197,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2974,7 +2968,7 @@
         <v>55</v>
       </c>
       <c r="C54" s="5"/>
-      <c r="D54" s="12" t="s">
+      <c r="D54" s="11" t="s">
         <v>96</v>
       </c>
       <c r="E54" s="4"/>
@@ -3562,8 +3556,8 @@
         <v>89</v>
       </c>
       <c r="C95" s="5"/>
-      <c r="D95" s="9" t="s">
-        <v>99</v>
+      <c r="D95" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="E95" s="4"/>
       <c r="F95" s="4"/>
@@ -3593,7 +3587,7 @@
       </c>
       <c r="D97" s="8">
         <f>COUNTIF(D3:D96,"identic")/$B$97</f>
-        <v>0.8936170212765957</v>
+        <v>0.9042553191489362</v>
       </c>
       <c r="E97" s="7"/>
       <c r="F97" s="8">
@@ -3642,10 +3636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3951,10 +3945,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>158</v>
+        <v>261</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="C21" s="22">
         <v>1</v>
@@ -3966,10 +3960,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C22" s="22">
         <v>1</v>
@@ -3981,10 +3975,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C23" s="22">
         <v>1</v>
@@ -3996,10 +3990,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C24" s="22">
         <v>1</v>
@@ -4011,10 +4005,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C25" s="22">
         <v>1</v>
@@ -4026,40 +4020,40 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="24">
-        <v>0</v>
+        <v>167</v>
+      </c>
+      <c r="C26" s="22">
+        <v>1</v>
+      </c>
+      <c r="D26" s="22">
+        <v>1</v>
       </c>
       <c r="E26" s="26"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C27" s="29"/>
-      <c r="D27" s="22">
-        <v>1</v>
+      <c r="D27" s="24">
+        <v>0</v>
       </c>
       <c r="E27" s="26"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="C28" s="22">
-        <v>1</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="C28" s="29"/>
       <c r="D28" s="22">
         <v>1</v>
       </c>
@@ -4067,25 +4061,25 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C29" s="22">
         <v>1</v>
       </c>
-      <c r="D29" s="28">
-        <v>0</v>
+      <c r="D29" s="22">
+        <v>1</v>
       </c>
       <c r="E29" s="26"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>176</v>
+        <v>263</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C30" s="22">
         <v>1</v>
@@ -4097,10 +4091,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C31" s="22">
         <v>1</v>
@@ -4112,10 +4106,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C32" s="22">
         <v>1</v>
@@ -4127,10 +4121,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C33" s="22">
         <v>1</v>
@@ -4142,10 +4136,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C34" s="22">
         <v>1</v>
@@ -4157,113 +4151,113 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>188</v>
-      </c>
-      <c r="D35" s="41"/>
+        <v>184</v>
+      </c>
+      <c r="C35" s="22">
+        <v>1</v>
+      </c>
+      <c r="D35" s="22">
+        <v>1</v>
+      </c>
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="C36" s="22">
-        <v>1</v>
-      </c>
-      <c r="D36" s="22">
-        <v>1</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="D36" s="41"/>
       <c r="E36" s="26"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C37" s="22">
         <v>1</v>
       </c>
-      <c r="D37" s="28">
-        <v>0</v>
+      <c r="D37" s="22">
+        <v>1</v>
       </c>
       <c r="E37" s="26"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C38" s="22">
         <v>1</v>
       </c>
-      <c r="D38" s="22">
-        <v>1</v>
+      <c r="D38" s="28">
+        <v>0</v>
       </c>
       <c r="E38" s="26"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C39" s="22">
         <v>1</v>
       </c>
-      <c r="D39" s="28">
-        <v>0</v>
+      <c r="D39" s="22">
+        <v>1</v>
       </c>
       <c r="E39" s="26"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C40" s="22">
         <v>1</v>
       </c>
-      <c r="D40" s="27">
-        <v>0.5</v>
+      <c r="D40" s="22">
+        <v>1</v>
       </c>
       <c r="E40" s="26"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="20" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C41" s="22">
         <v>1</v>
       </c>
-      <c r="D41" s="22">
-        <v>1</v>
+      <c r="D41" s="27">
+        <v>0.5</v>
       </c>
       <c r="E41" s="26"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C42" s="22">
         <v>1</v>
@@ -4275,71 +4269,71 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C43" s="22">
         <v>1</v>
       </c>
-      <c r="D43" s="28">
-        <v>0</v>
+      <c r="D43" s="22">
+        <v>1</v>
       </c>
       <c r="E43" s="26"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="C44" s="22">
+        <v>1</v>
+      </c>
+      <c r="D44" s="28">
+        <v>0</v>
+      </c>
+      <c r="E44" s="26"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="B45" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="B44" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="22">
-        <v>1</v>
-      </c>
-      <c r="E44" s="26"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="20"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="22">
+        <v>1</v>
+      </c>
       <c r="E45" s="26"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="20"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="26"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="B46" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="19"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>208</v>
-      </c>
-      <c r="C47" s="22">
-        <v>1</v>
-      </c>
-      <c r="D47" s="22">
-        <v>1</v>
-      </c>
-      <c r="E47" s="26"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="19"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C48" s="22">
         <v>1</v>
@@ -4351,10 +4345,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C49" s="22">
         <v>1</v>
@@ -4366,10 +4360,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C50" s="22">
         <v>1</v>
@@ -4381,10 +4375,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C51" s="22">
         <v>1</v>
@@ -4396,10 +4390,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C52" s="22">
         <v>1</v>
@@ -4411,10 +4405,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C53" s="22">
         <v>1</v>
@@ -4426,10 +4420,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C54" s="22">
         <v>1</v>
@@ -4441,94 +4435,94 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="20" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B55" s="21" t="s">
-        <v>224</v>
-      </c>
-      <c r="C55" s="27">
-        <v>0.75</v>
+        <v>221</v>
+      </c>
+      <c r="C55" s="22">
+        <v>1</v>
       </c>
       <c r="D55" s="22">
         <v>1</v>
       </c>
-      <c r="E55" s="26" t="s">
-        <v>225</v>
-      </c>
+      <c r="E55" s="26"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C56" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="D56" s="22">
+        <v>1</v>
+      </c>
+      <c r="E56" s="26" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="B57" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="B56" s="21" t="s">
+      <c r="C57" s="22">
+        <v>1</v>
+      </c>
+      <c r="D57" s="22">
+        <v>1</v>
+      </c>
+      <c r="E57" s="26"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="C56" s="22">
-        <v>1</v>
-      </c>
-      <c r="D56" s="22">
-        <v>1</v>
-      </c>
-      <c r="E56" s="26"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="31" t="s">
+      <c r="B58" s="26"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="26"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="B57" s="26"/>
-      <c r="C57" s="30"/>
-      <c r="D57" s="30"/>
-      <c r="E57" s="26"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="16" t="s">
+      <c r="B59" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="B58" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="19"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="B59" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="C59" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="D59" s="28">
-        <v>0</v>
-      </c>
-      <c r="E59" s="26" t="s">
-        <v>233</v>
-      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="19"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B60" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="C60" s="22">
-        <v>1</v>
-      </c>
-      <c r="D60" s="24">
+        <v>231</v>
+      </c>
+      <c r="C60" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="D60" s="28">
         <v>0</v>
       </c>
-      <c r="E60" s="26"/>
+      <c r="E60" s="26" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C61" s="22">
         <v>1</v>
@@ -4540,10 +4534,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B62" s="21" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C62" s="22">
         <v>1</v>
@@ -4555,10 +4549,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B63" s="21" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C63" s="22">
         <v>1</v>
@@ -4570,10 +4564,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B64" s="21" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C64" s="22">
         <v>1</v>
@@ -4585,113 +4579,128 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B65" s="21" t="s">
-        <v>245</v>
-      </c>
-      <c r="C65" s="27">
-        <v>0.75</v>
+        <v>242</v>
+      </c>
+      <c r="C65" s="22">
+        <v>1</v>
       </c>
       <c r="D65" s="24">
         <v>0</v>
       </c>
-      <c r="E65" s="26" t="s">
-        <v>246</v>
-      </c>
+      <c r="E65" s="26"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B66" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="C66" s="22">
-        <v>1</v>
+        <v>244</v>
+      </c>
+      <c r="C66" s="27">
+        <v>0.75</v>
       </c>
       <c r="D66" s="24">
         <v>0</v>
       </c>
-      <c r="E66" s="26"/>
+      <c r="E66" s="26" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="20" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B67" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="26" t="s">
-        <v>251</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="C67" s="22">
+        <v>1</v>
+      </c>
+      <c r="D67" s="24">
+        <v>0</v>
+      </c>
+      <c r="E67" s="26"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="20" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B68" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="C68" s="22">
-        <v>1</v>
-      </c>
-      <c r="D68" s="24">
-        <v>0</v>
-      </c>
-      <c r="E68" s="26"/>
+        <v>249</v>
+      </c>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="26" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="C69" s="22">
+        <v>1</v>
+      </c>
+      <c r="D69" s="24">
+        <v>0</v>
+      </c>
+      <c r="E69" s="26"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="B70" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="B69" s="21" t="s">
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="C69" s="29"/>
-      <c r="D69" s="29"/>
-      <c r="E69" s="26" t="s">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="31" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="31" t="s">
+      <c r="B71" s="26"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="26"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="B70" s="26"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="33"/>
-      <c r="E70" s="26"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="16" t="s">
+      <c r="B72" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="B71" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="C71" s="22">
-        <v>1</v>
-      </c>
-      <c r="D71" s="24">
+      <c r="C72" s="22">
+        <v>1</v>
+      </c>
+      <c r="D72" s="24">
         <v>0</v>
       </c>
-      <c r="E71" s="19"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="34"/>
-      <c r="B72" s="35"/>
-      <c r="C72" s="36">
-        <f>AVERAGE(C3:C71)</f>
-        <v>0.98947368421052628</v>
-      </c>
-      <c r="D72" s="36">
-        <f>AVERAGE(D3:D71)</f>
-        <v>0.6791666666666667</v>
-      </c>
-      <c r="E72" s="35"/>
+      <c r="E72" s="19"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="34"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="36">
+        <f>AVERAGE(C3:C72)</f>
+        <v>0.98965517241379308</v>
+      </c>
+      <c r="D73" s="36">
+        <f>AVERAGE(D3:D72)</f>
+        <v>0.71721311475409832</v>
+      </c>
+      <c r="E73" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4699,7 +4708,7 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor refactoring and synchronization of GKv3
</commit_message>
<xml_diff>
--- a/dev_info/gk_compatibility_matrix.xlsx
+++ b/dev_info/gk_compatibility_matrix.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKS\shared\gkdev\GEDKeeper\dev_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290D95D4-D891-4D15-96A4-370E17A0EEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C86A9E5-1C7A-4ED6-841C-09587E72FC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compatibility Matrix" sheetId="2" r:id="rId1"/>
-    <sheet name="Linux(Mono) Status" sheetId="3" r:id="rId2"/>
+    <sheet name="problems" sheetId="4" r:id="rId2"/>
+    <sheet name="Linux(Mono) Status" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Compatibility Matrix'!$A$2:$F$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Compatibility Matrix'!$A$2:$G$96</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -214,7 +215,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="316">
   <si>
     <t>Module</t>
   </si>
@@ -1050,6 +1051,162 @@
   </si>
   <si>
     <t>1.20.1</t>
+  </si>
+  <si>
+    <t>Last Sync</t>
+  </si>
+  <si>
+    <t>CustomChart</t>
+  </si>
+  <si>
+    <t>CircleChart</t>
+  </si>
+  <si>
+    <t>центрирование и масштаб - проверить, клавиши зума - могут не работать, потом синк - заново</t>
+  </si>
+  <si>
+    <t>клавиши, мышка, печать - проверить</t>
+  </si>
+  <si>
+    <t>FilterGridView</t>
+  </si>
+  <si>
+    <t>проверить весь функционал</t>
+  </si>
+  <si>
+    <t>TreeChartBox</t>
+  </si>
+  <si>
+    <t>проверить клавиши, мышку, печать, границы, зум, скролл, восстановить бэкграунд изображение</t>
+  </si>
+  <si>
+    <t>в GKv2 неправильно работает субконтрол поколений</t>
+  </si>
+  <si>
+    <t>AppHost</t>
+  </si>
+  <si>
+    <t>как сохранять последние файлы при SDI интерфейсе (закрытие окон по одному)?</t>
+  </si>
+  <si>
+    <t>GKProgram</t>
+  </si>
+  <si>
+    <t>нет поддержки единственного экземпляра</t>
+  </si>
+  <si>
+    <t>MediaViewerWin</t>
+  </si>
+  <si>
+    <t>проблемы с просмотром изображений при открытии окна</t>
+  </si>
+  <si>
+    <t>BaseWinSDI</t>
+  </si>
+  <si>
+    <t>выпадающий список (меню) последних файлов</t>
+  </si>
+  <si>
+    <t>NoteEditDlgEx</t>
+  </si>
+  <si>
+    <t>выпадающий список (меню) или комбобокс размеров шрифта?</t>
+  </si>
+  <si>
+    <t>PersonEditDlg</t>
+  </si>
+  <si>
+    <t>очень корявый вид. Почему?</t>
+  </si>
+  <si>
+    <t>PortraitSelectDlg</t>
+  </si>
+  <si>
+    <t>ProgressDlg</t>
+  </si>
+  <si>
+    <t>не работает</t>
+  </si>
+  <si>
+    <t>SlideshowWin</t>
+  </si>
+  <si>
+    <t>TreeChartWin</t>
+  </si>
+  <si>
+    <t>для чего перетаскивание? Не работает фоновое изображение</t>
+  </si>
+  <si>
+    <t>ArborViewer</t>
+  </si>
+  <si>
+    <t>линии без стрелок</t>
+  </si>
+  <si>
+    <t>ControlHandlers</t>
+  </si>
+  <si>
+    <t>сверить функционал</t>
+  </si>
+  <si>
+    <t>WFGfxProvider</t>
+  </si>
+  <si>
+    <t>прозрачность загружаемых ресурсных изображений</t>
+  </si>
+  <si>
+    <t>WFGfxRenderer</t>
+  </si>
+  <si>
+    <t>прозрачность выводимых изображений</t>
+  </si>
+  <si>
+    <t>ZGraphControl</t>
+  </si>
+  <si>
+    <t>названия осей, корректность вывода данных</t>
+  </si>
+  <si>
+    <t>WizardPages</t>
+  </si>
+  <si>
+    <t>нужна альтернативная реализация</t>
+  </si>
+  <si>
+    <t>UIHelper</t>
+  </si>
+  <si>
+    <t>мелкие нестыковки, исправление по ходу адаптации порта</t>
+  </si>
+  <si>
+    <t>GKPortrait</t>
+  </si>
+  <si>
+    <t>не работает слайд-панель кнопок</t>
+  </si>
+  <si>
+    <t>GKTabControl</t>
+  </si>
+  <si>
+    <t>не реализовано отображение иконок и закрытие табов</t>
+  </si>
+  <si>
+    <t>ImageBox</t>
+  </si>
+  <si>
+    <t>множество мелких нестыковок и несовпадений с неизвестным эффектом, возможно нужно урезать ненужный функционал wf-варианта</t>
+  </si>
+  <si>
+    <t>ScrollablePanel</t>
+  </si>
+  <si>
+    <t>множество мелких нестыковок и несовпадений с неизвестным эффектом</t>
+  </si>
+  <si>
+    <t>MediaPlayer</t>
+  </si>
+  <si>
+    <t>множество неработающих функций</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1655,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1652,6 +1809,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1700,7 +1901,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1788,6 +1989,24 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1796,6 +2015,9 @@
     </xf>
     <xf numFmtId="2" fontId="16" fillId="41" borderId="12" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -2193,58 +2415,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38" t="s">
+      <c r="D1" s="43"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="38"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="38"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="41"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2255,10 +2482,11 @@
       <c r="D3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2271,10 +2499,11 @@
       <c r="D4" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="37"/>
       <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -2285,10 +2514,11 @@
       <c r="D5" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2299,10 +2529,11 @@
       <c r="D6" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -2313,10 +2544,11 @@
       <c r="D7" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="37"/>
       <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -2327,10 +2559,11 @@
       <c r="D8" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="4"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -2341,10 +2574,11 @@
       <c r="D9" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -2355,10 +2589,11 @@
       <c r="D10" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="37"/>
       <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -2369,10 +2604,11 @@
       <c r="D11" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -2383,10 +2619,11 @@
       <c r="D12" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -2397,10 +2634,11 @@
       <c r="D13" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -2411,10 +2649,11 @@
       <c r="D14" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -2425,10 +2664,11 @@
       <c r="D15" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -2439,10 +2679,11 @@
       <c r="D16" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -2453,10 +2694,11 @@
       <c r="D17" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -2467,10 +2709,11 @@
       <c r="D18" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="11"/>
       <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -2481,10 +2724,11 @@
       <c r="D19" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="11"/>
       <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -2495,10 +2739,11 @@
       <c r="D20" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="11"/>
       <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -2509,10 +2754,11 @@
       <c r="D21" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="11"/>
       <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -2523,10 +2769,11 @@
       <c r="D22" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="11"/>
       <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
@@ -2537,10 +2784,11 @@
       <c r="D23" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="11"/>
       <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -2551,10 +2799,11 @@
       <c r="D24" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="11"/>
       <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>2</v>
       </c>
@@ -2565,10 +2814,11 @@
       <c r="D25" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="11"/>
       <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>2</v>
       </c>
@@ -2579,10 +2829,11 @@
       <c r="D26" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="11"/>
       <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>2</v>
       </c>
@@ -2593,10 +2844,11 @@
       <c r="D27" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="11"/>
       <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>2</v>
       </c>
@@ -2607,10 +2859,11 @@
       <c r="D28" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="11"/>
       <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
@@ -2621,10 +2874,11 @@
       <c r="D29" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="37"/>
       <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>2</v>
       </c>
@@ -2635,10 +2889,11 @@
       <c r="D30" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="11"/>
       <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>2</v>
       </c>
@@ -2649,10 +2904,11 @@
       <c r="D31" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="11"/>
       <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>2</v>
       </c>
@@ -2663,10 +2919,11 @@
       <c r="D32" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>2</v>
       </c>
@@ -2677,10 +2934,11 @@
       <c r="D33" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="11"/>
       <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>2</v>
       </c>
@@ -2691,10 +2949,11 @@
       <c r="D34" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="11"/>
       <c r="F34" s="4"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>2</v>
       </c>
@@ -2705,10 +2964,11 @@
       <c r="D35" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="11"/>
       <c r="F35" s="4"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
@@ -2719,10 +2979,11 @@
       <c r="D36" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="11"/>
       <c r="F36" s="4"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" s="4"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>2</v>
       </c>
@@ -2733,10 +2994,11 @@
       <c r="D37" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E37" s="4"/>
+      <c r="E37" s="11"/>
       <c r="F37" s="4"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>2</v>
       </c>
@@ -2747,10 +3009,11 @@
       <c r="D38" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="37"/>
       <c r="F38" s="4"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>2</v>
       </c>
@@ -2761,10 +3024,11 @@
       <c r="D39" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="11"/>
       <c r="F39" s="4"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>2</v>
       </c>
@@ -2775,10 +3039,11 @@
       <c r="D40" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E40" s="4"/>
+      <c r="E40" s="10"/>
       <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" s="4"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>2</v>
       </c>
@@ -2789,10 +3054,11 @@
       <c r="D41" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="11"/>
       <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>2</v>
       </c>
@@ -2803,10 +3069,11 @@
       <c r="D42" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E42" s="4"/>
+      <c r="E42" s="10"/>
       <c r="F42" s="4"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" s="4"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -2817,10 +3084,11 @@
       <c r="D43" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="11"/>
       <c r="F43" s="4"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" s="4"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>2</v>
       </c>
@@ -2831,10 +3099,11 @@
       <c r="D44" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E44" s="4"/>
+      <c r="E44" s="11"/>
       <c r="F44" s="4"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" s="4"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>2</v>
       </c>
@@ -2845,10 +3114,11 @@
       <c r="D45" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E45" s="4"/>
+      <c r="E45" s="11"/>
       <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>2</v>
       </c>
@@ -2859,10 +3129,11 @@
       <c r="D46" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E46" s="4"/>
+      <c r="E46" s="11"/>
       <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" s="4"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>2</v>
       </c>
@@ -2873,10 +3144,11 @@
       <c r="D47" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="4"/>
+      <c r="E47" s="11"/>
       <c r="F47" s="4"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" s="4"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>2</v>
       </c>
@@ -2887,10 +3159,11 @@
       <c r="D48" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E48" s="4"/>
+      <c r="E48" s="11"/>
       <c r="F48" s="4"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" s="4"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>2</v>
       </c>
@@ -2901,10 +3174,11 @@
       <c r="D49" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E49" s="4"/>
+      <c r="E49" s="11"/>
       <c r="F49" s="4"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>2</v>
       </c>
@@ -2915,10 +3189,11 @@
       <c r="D50" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E50" s="4"/>
+      <c r="E50" s="11"/>
       <c r="F50" s="4"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>2</v>
       </c>
@@ -2929,10 +3204,11 @@
       <c r="D51" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E51" s="4"/>
+      <c r="E51" s="10"/>
       <c r="F51" s="4"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>2</v>
       </c>
@@ -2943,10 +3219,11 @@
       <c r="D52" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E52" s="4"/>
+      <c r="E52" s="11"/>
       <c r="F52" s="4"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" s="4"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>2</v>
       </c>
@@ -2957,10 +3234,11 @@
       <c r="D53" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E53" s="4"/>
+      <c r="E53" s="11"/>
       <c r="F53" s="4"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" s="4"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>2</v>
       </c>
@@ -2971,10 +3249,11 @@
       <c r="D54" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E54" s="4"/>
+      <c r="E54" s="11"/>
       <c r="F54" s="4"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54" s="4"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>2</v>
       </c>
@@ -2985,10 +3264,11 @@
       <c r="D55" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E55" s="4"/>
+      <c r="E55" s="11"/>
       <c r="F55" s="4"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55" s="4"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>2</v>
       </c>
@@ -2999,10 +3279,11 @@
       <c r="D56" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E56" s="4"/>
+      <c r="E56" s="11"/>
       <c r="F56" s="4"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56" s="4"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>2</v>
       </c>
@@ -3013,10 +3294,11 @@
       <c r="D57" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E57" s="4"/>
+      <c r="E57" s="37"/>
       <c r="F57" s="4"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57" s="4"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>2</v>
       </c>
@@ -3027,10 +3309,11 @@
       <c r="D58" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E58" s="4"/>
+      <c r="E58" s="11"/>
       <c r="F58" s="4"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58" s="4"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>2</v>
       </c>
@@ -3041,10 +3324,11 @@
       <c r="D59" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E59" s="4"/>
+      <c r="E59" s="11"/>
       <c r="F59" s="4"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59" s="4"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>2</v>
       </c>
@@ -3055,10 +3339,11 @@
       <c r="D60" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E60" s="4"/>
+      <c r="E60" s="11"/>
       <c r="F60" s="4"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60" s="4"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>2</v>
       </c>
@@ -3069,10 +3354,11 @@
       <c r="D61" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E61" s="4"/>
+      <c r="E61" s="11"/>
       <c r="F61" s="4"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61" s="4"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>2</v>
       </c>
@@ -3083,10 +3369,11 @@
       <c r="D62" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E62" s="4"/>
+      <c r="E62" s="11"/>
       <c r="F62" s="4"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62" s="4"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>2</v>
       </c>
@@ -3097,10 +3384,11 @@
       <c r="D63" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E63" s="4"/>
+      <c r="E63" s="11"/>
       <c r="F63" s="4"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63" s="4"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>2</v>
       </c>
@@ -3111,10 +3399,11 @@
       <c r="D64" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E64" s="4"/>
+      <c r="E64" s="11"/>
       <c r="F64" s="4"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64" s="4"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>2</v>
       </c>
@@ -3125,10 +3414,11 @@
       <c r="D65" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E65" s="4"/>
+      <c r="E65" s="11"/>
       <c r="F65" s="4"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65" s="4"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>2</v>
       </c>
@@ -3139,10 +3429,11 @@
       <c r="D66" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E66" s="4"/>
+      <c r="E66" s="11"/>
       <c r="F66" s="4"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66" s="4"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>2</v>
       </c>
@@ -3153,10 +3444,11 @@
       <c r="D67" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E67" s="4"/>
+      <c r="E67" s="11"/>
       <c r="F67" s="4"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G67" s="4"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>3</v>
       </c>
@@ -3167,10 +3459,11 @@
       <c r="D68" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E68" s="4"/>
+      <c r="E68" s="37"/>
       <c r="F68" s="4"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68" s="4"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>3</v>
       </c>
@@ -3181,10 +3474,11 @@
       <c r="D69" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E69" s="4"/>
+      <c r="E69" s="37"/>
       <c r="F69" s="4"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69" s="4"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>3</v>
       </c>
@@ -3195,10 +3489,11 @@
       <c r="D70" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E70" s="4"/>
+      <c r="E70" s="11"/>
       <c r="F70" s="4"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70" s="4"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>3</v>
       </c>
@@ -3209,10 +3504,11 @@
       <c r="D71" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E71" s="4"/>
+      <c r="E71" s="11"/>
       <c r="F71" s="4"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71" s="4"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>3</v>
       </c>
@@ -3223,10 +3519,11 @@
       <c r="D72" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E72" s="4"/>
+      <c r="E72" s="11"/>
       <c r="F72" s="4"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G72" s="4"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>3</v>
       </c>
@@ -3237,10 +3534,11 @@
       <c r="D73" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E73" s="4"/>
+      <c r="E73" s="11"/>
       <c r="F73" s="4"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73" s="4"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>3</v>
       </c>
@@ -3251,10 +3549,11 @@
       <c r="D74" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E74" s="4"/>
+      <c r="E74" s="39"/>
       <c r="F74" s="4"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74" s="4"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>3</v>
       </c>
@@ -3265,10 +3564,11 @@
       <c r="D75" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E75" s="4"/>
+      <c r="E75" s="11"/>
       <c r="F75" s="4"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G75" s="4"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>3</v>
       </c>
@@ -3281,10 +3581,11 @@
       <c r="D76" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E76" s="4"/>
+      <c r="E76" s="6"/>
       <c r="F76" s="4"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G76" s="4"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>3</v>
       </c>
@@ -3295,10 +3596,11 @@
       <c r="D77" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E77" s="4"/>
+      <c r="E77" s="37"/>
       <c r="F77" s="4"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G77" s="4"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>3</v>
       </c>
@@ -3309,10 +3611,11 @@
       <c r="D78" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E78" s="4"/>
+      <c r="E78" s="11"/>
       <c r="F78" s="4"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G78" s="4"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>3</v>
       </c>
@@ -3323,10 +3626,11 @@
       <c r="D79" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E79" s="4"/>
+      <c r="E79" s="12"/>
       <c r="F79" s="4"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G79" s="4"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>3</v>
       </c>
@@ -3337,10 +3641,11 @@
       <c r="D80" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E80" s="4"/>
+      <c r="E80" s="11"/>
       <c r="F80" s="4"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80" s="4"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>3</v>
       </c>
@@ -3351,10 +3656,11 @@
       <c r="D81" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E81" s="4"/>
+      <c r="E81" s="11"/>
       <c r="F81" s="4"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G81" s="4"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>3</v>
       </c>
@@ -3365,10 +3671,11 @@
       <c r="D82" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E82" s="4"/>
+      <c r="E82" s="10"/>
       <c r="F82" s="4"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82" s="4"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>3</v>
       </c>
@@ -3379,10 +3686,11 @@
       <c r="D83" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E83" s="4"/>
+      <c r="E83" s="11"/>
       <c r="F83" s="4"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G83" s="4"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>3</v>
       </c>
@@ -3393,10 +3701,11 @@
       <c r="D84" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E84" s="4"/>
+      <c r="E84" s="11"/>
       <c r="F84" s="4"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G84" s="4"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>3</v>
       </c>
@@ -3407,10 +3716,11 @@
       <c r="D85" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E85" s="4"/>
+      <c r="E85" s="10"/>
       <c r="F85" s="4"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G85" s="4"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>3</v>
       </c>
@@ -3423,10 +3733,11 @@
       <c r="D86" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="E86" s="4"/>
+      <c r="E86" s="6"/>
       <c r="F86" s="4"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G86" s="4"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>3</v>
       </c>
@@ -3437,10 +3748,11 @@
       <c r="D87" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E87" s="4"/>
+      <c r="E87" s="10"/>
       <c r="F87" s="4"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G87" s="4"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>3</v>
       </c>
@@ -3451,10 +3763,11 @@
       <c r="D88" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E88" s="4"/>
+      <c r="E88" s="37"/>
       <c r="F88" s="4"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G88" s="4"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>3</v>
       </c>
@@ -3467,10 +3780,11 @@
       <c r="D89" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E89" s="4"/>
+      <c r="E89" s="37"/>
       <c r="F89" s="4"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G89" s="4"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>3</v>
       </c>
@@ -3483,10 +3797,11 @@
       <c r="D90" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E90" s="4"/>
+      <c r="E90" s="37"/>
       <c r="F90" s="4"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G90" s="4"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>3</v>
       </c>
@@ -3499,10 +3814,11 @@
       <c r="D91" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E91" s="4"/>
+      <c r="E91" s="6"/>
       <c r="F91" s="4"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G91" s="4"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>3</v>
       </c>
@@ -3515,10 +3831,11 @@
       <c r="D92" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E92" s="4"/>
+      <c r="E92" s="11"/>
       <c r="F92" s="4"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G92" s="4"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>3</v>
       </c>
@@ -3531,10 +3848,11 @@
       <c r="D93" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E93" s="4"/>
+      <c r="E93" s="11"/>
       <c r="F93" s="4"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G93" s="4"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>3</v>
       </c>
@@ -3545,10 +3863,11 @@
       <c r="D94" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E94" s="4"/>
+      <c r="E94" s="48"/>
       <c r="F94" s="4"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G94" s="4"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>3</v>
       </c>
@@ -3559,10 +3878,11 @@
       <c r="D95" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E95" s="4"/>
+      <c r="E95" s="37"/>
       <c r="F95" s="4"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95" s="4"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>3</v>
       </c>
@@ -3573,10 +3893,11 @@
       <c r="D96" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E96" s="4"/>
+      <c r="E96" s="11"/>
       <c r="F96" s="4"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G96" s="4"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="7"/>
       <c r="B97" s="7">
         <f>COUNTA(B3:B96)</f>
@@ -3589,13 +3910,14 @@
         <f>COUNTIF(D3:D96,"identic")/$B$97</f>
         <v>0.9042553191489362</v>
       </c>
-      <c r="E97" s="7"/>
-      <c r="F97" s="8">
-        <f>COUNTIF(F3:F96,"identic")/$B$97</f>
+      <c r="E97" s="8"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="8">
+        <f>COUNTIF(G3:G96,"identic")/$B$97</f>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7" t="s">
@@ -3605,28 +3927,29 @@
         <f>COUNTA(D3:D96)/$B$97</f>
         <v>1</v>
       </c>
-      <c r="E98" s="7"/>
-      <c r="F98" s="8">
-        <f>COUNTA(F3:F96)/$B$97</f>
+      <c r="E98" s="8"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="8">
+        <f>COUNTA(G3:G96)/$B$97</f>
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F96" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:G96" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3635,11 +3958,243 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D03122-1CE5-4F45-B81F-5C9B25195EE8}">
+  <dimension ref="B2:C28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="122.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>282</v>
+      </c>
+      <c r="C11" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>284</v>
+      </c>
+      <c r="C12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>289</v>
+      </c>
+      <c r="C15" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>290</v>
+      </c>
+      <c r="C16" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>292</v>
+      </c>
+      <c r="C17" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>296</v>
+      </c>
+      <c r="C19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>298</v>
+      </c>
+      <c r="C20" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>300</v>
+      </c>
+      <c r="C21" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>302</v>
+      </c>
+      <c r="C22" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>304</v>
+      </c>
+      <c r="C23" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>306</v>
+      </c>
+      <c r="C24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>308</v>
+      </c>
+      <c r="C25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>310</v>
+      </c>
+      <c r="C26" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>312</v>
+      </c>
+      <c r="C27" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>314</v>
+      </c>
+      <c r="C28" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3652,30 +4207,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
       <c r="C2" s="15" t="s">
         <v>120</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="39"/>
+      <c r="E2" s="45"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
@@ -4171,10 +4726,10 @@
       <c r="B36" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="D36" s="41"/>
+      <c r="D36" s="47"/>
       <c r="E36" s="26"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
GKv3: fixed work of ImageBox and dependent MediaViewerWin, PortraitSelectDlg, SlideshowWin
</commit_message>
<xml_diff>
--- a/dev_info/gk_compatibility_matrix.xlsx
+++ b/dev_info/gk_compatibility_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKS\shared\gkdev\GEDKeeper\dev_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C86A9E5-1C7A-4ED6-841C-09587E72FC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E86BABF-2964-43A1-9DB5-858BC49BC78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,6 @@
     <author>tc={B204A590-8F59-45C2-AF46-0C451D79A7F2}</author>
     <author>tc={CABCC935-D353-49C6-BF7B-26945C3B7EEC}</author>
     <author>tc={4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}</author>
-    <author>tc={2E4E5FAA-8920-4E1D-B04E-22732D846631}</author>
     <author>tc={BD118A23-46B1-45EB-A479-612E3372B34F}</author>
     <author>tc={34F4FF22-A13C-482B-B521-D1FCFDCF8C10}</author>
     <author>tc={D1AD9B46-69A2-4F81-ADD4-0B51A5891E85}</author>
@@ -90,15 +89,7 @@
     require toolbar's combobox and dropdownbtn</t>
       </text>
     </comment>
-    <comment ref="D51" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <t>[Цепочка примечаний]
-Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
-Комментарий:
-    first image not fitted to window</t>
-      </text>
-    </comment>
-    <comment ref="D68" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="D68" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <t>[Цепочка примечаний]
 Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
@@ -106,7 +97,7 @@
     lines without arrow's caps</t>
       </text>
     </comment>
-    <comment ref="D74" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="D74" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <t>[Цепочка примечаний]
 Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
@@ -114,7 +105,7 @@
     many errors and dont work sorting</t>
       </text>
     </comment>
-    <comment ref="D77" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="D77" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <t>[Цепочка примечаний]
 Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
@@ -215,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="312">
   <si>
     <t>Module</t>
   </si>
@@ -1095,12 +1086,6 @@
     <t>нет поддержки единственного экземпляра</t>
   </si>
   <si>
-    <t>MediaViewerWin</t>
-  </si>
-  <si>
-    <t>проблемы с просмотром изображений при открытии окна</t>
-  </si>
-  <si>
     <t>BaseWinSDI</t>
   </si>
   <si>
@@ -1119,16 +1104,10 @@
     <t>очень корявый вид. Почему?</t>
   </si>
   <si>
-    <t>PortraitSelectDlg</t>
-  </si>
-  <si>
     <t>ProgressDlg</t>
   </si>
   <si>
     <t>не работает</t>
-  </si>
-  <si>
-    <t>SlideshowWin</t>
   </si>
   <si>
     <t>TreeChartWin</t>
@@ -1995,6 +1974,9 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2015,9 +1997,6 @@
     </xf>
     <xf numFmtId="2" fontId="16" fillId="41" borderId="12" xfId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -2398,9 +2377,6 @@
   <threadedComment ref="D32" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{4EDC0CEC-EFA2-43F9-A0AF-C90394B6A235}">
     <text>require toolbar's combobox and dropdownbtn</text>
   </threadedComment>
-  <threadedComment ref="D51" dT="2021-05-07T20:09:13.00" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{2E4E5FAA-8920-4E1D-B04E-22732D846631}">
-    <text>first image not fitted to window</text>
-  </threadedComment>
   <threadedComment ref="D68" dT="2021-05-07T19:42:23.30" personId="{8F280277-BD00-4959-B18B-5943571B3E6B}" id="{BD118A23-46B1-45EB-A479-612E3372B34F}">
     <text>lines without arrow's caps</text>
   </threadedComment>
@@ -2418,40 +2394,40 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B85" sqref="B85"/>
+      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.21875" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="43"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="41" t="s">
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="41"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
+      <c r="A2" s="42"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2874,7 +2850,7 @@
       <c r="D29" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="37"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
@@ -3039,7 +3015,7 @@
       <c r="D40" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E40" s="10"/>
+      <c r="E40" s="11"/>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
@@ -3201,10 +3177,10 @@
         <v>52</v>
       </c>
       <c r="C51" s="5"/>
-      <c r="D51" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="E51" s="10"/>
+      <c r="D51" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51" s="11"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
     </row>
@@ -3668,10 +3644,10 @@
         <v>82</v>
       </c>
       <c r="C82" s="5"/>
-      <c r="D82" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E82" s="10"/>
+      <c r="D82" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="E82" s="37"/>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
     </row>
@@ -3863,7 +3839,7 @@
       <c r="D94" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E94" s="48"/>
+      <c r="E94" s="41"/>
       <c r="F94" s="4"/>
       <c r="G94" s="4"/>
     </row>
@@ -3959,10 +3935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D03122-1CE5-4F45-B81F-5C9B25195EE8}">
-  <dimension ref="B2:C28"/>
+  <dimension ref="B2:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4026,18 +4002,18 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C10" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
@@ -4061,127 +4037,103 @@
         <v>286</v>
       </c>
       <c r="C13" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C14" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C15" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C16" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C17" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C18" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C19" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C20" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C21" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C22" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C23" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C24" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C25" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
-        <v>310</v>
-      </c>
-      <c r="C26" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>312</v>
-      </c>
-      <c r="C27" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>314</v>
-      </c>
-      <c r="C28" t="s">
-        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -4207,30 +4159,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45" t="s">
+      <c r="D1" s="46"/>
+      <c r="E1" s="46" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
       <c r="C2" s="15" t="s">
         <v>120</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="45"/>
+      <c r="E2" s="46"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
@@ -4726,10 +4678,10 @@
       <c r="B36" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="C36" s="46" t="s">
+      <c r="C36" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="D36" s="47"/>
+      <c r="D36" s="48"/>
       <c r="E36" s="26"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
GKv3: migration of ProgressDlg, TreeChartWin, TTPatSearchDlg, TTTreeMergeDlg (#382)
</commit_message>
<xml_diff>
--- a/dev_info/gk_compatibility_matrix.xlsx
+++ b/dev_info/gk_compatibility_matrix.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKS\shared\gkdev\GEDKeeper\dev_info\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848059A3-F8A7-4D01-A457-212E355A9068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compatibility Matrix" sheetId="2" r:id="rId1"/>
@@ -13,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Compatibility Matrix'!$A$2:$G$98</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,27 +36,17 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={B204A590-8F59-45C2-AF46-0C451D79A7F2}</author>
   </authors>
   <commentList>
-    <comment ref="D10" authorId="0">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <charset val="204"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Цепочка примечаний]
+        <t>[Цепочка примечаний]
 Ваша версия Excel позволяет прочитать эту цепочку примечаний, но если открыть файл в более поздней версии Excel, все внесенные в нее изменения будут удалены. Подробнее: https://go.microsoft.com/fwlink/?linkid=870924
 Комментарий:
     many small inaccuracies</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -58,12 +54,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="D14" authorId="0">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +85,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D15" authorId="0">
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0">
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="276">
   <si>
     <t>Module</t>
   </si>
@@ -971,9 +967,6 @@
   </si>
   <si>
     <t>everywhere (2/3) the subcontrol of generations does not work correctly</t>
-  </si>
-  <si>
-    <t>looks ugly</t>
   </si>
   <si>
     <t>player fills the entire window</t>
@@ -982,7 +975,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -1721,24 +1714,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="45">
-    <cellStyle name="20% - Акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Акцент1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Акцент2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Акцент3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -1757,12 +1750,12 @@
     <cellStyle name="Название" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Нейтральный" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="43"/>
+    <cellStyle name="Обычный 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
     <cellStyle name="Плохой" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Пояснение" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Примечание" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Процентный" xfId="42" builtinId="5"/>
-    <cellStyle name="Процентный 2" xfId="44"/>
+    <cellStyle name="Процентный 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
     <cellStyle name="Связанная ячейка" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Текст предупреждения" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Хороший" xfId="6" builtinId="26" customBuiltin="1"/>
@@ -2075,7 +2068,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2090,26 +2083,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="66" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>1</v>
       </c>
@@ -2126,7 +2119,7 @@
       </c>
       <c r="G1" s="37"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="37"/>
       <c r="B2" s="35" t="s">
         <v>0</v>
@@ -2147,7 +2140,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2164,7 +2157,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -2183,7 +2176,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -2198,7 +2191,7 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2215,7 +2208,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2232,7 +2225,7 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -2247,7 +2240,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -2262,7 +2255,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -2279,7 +2272,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -2294,7 +2287,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
@@ -2309,7 +2302,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -2324,7 +2317,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -2341,7 +2334,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -2356,7 +2349,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -2371,7 +2364,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -2386,7 +2379,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -2401,7 +2394,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
@@ -2416,7 +2409,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -2433,7 +2426,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -2448,7 +2441,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -2463,7 +2456,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -2478,7 +2471,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -2493,7 +2486,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
@@ -2508,7 +2501,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
@@ -2523,7 +2516,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
@@ -2538,7 +2531,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2553,7 +2546,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>2</v>
       </c>
@@ -2568,7 +2561,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
@@ -2583,7 +2576,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
@@ -2598,7 +2591,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>2</v>
       </c>
@@ -2615,7 +2608,7 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>2</v>
       </c>
@@ -2630,7 +2623,7 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
@@ -2645,7 +2638,7 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
@@ -2660,7 +2653,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
@@ -2675,7 +2668,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>2</v>
       </c>
@@ -2690,7 +2683,7 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -2698,16 +2691,14 @@
         <v>39</v>
       </c>
       <c r="C38" s="4"/>
-      <c r="D38" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="36" t="s">
-        <v>275</v>
-      </c>
+      <c r="D38" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="36"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -2722,7 +2713,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>2</v>
       </c>
@@ -2737,7 +2728,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>2</v>
       </c>
@@ -2752,7 +2743,7 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>2</v>
       </c>
@@ -2767,7 +2758,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
@@ -2782,7 +2773,7 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>2</v>
       </c>
@@ -2797,7 +2788,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
@@ -2812,7 +2803,7 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>2</v>
       </c>
@@ -2827,7 +2818,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>2</v>
       </c>
@@ -2842,7 +2833,7 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
@@ -2857,7 +2848,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
@@ -2872,7 +2863,7 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>2</v>
       </c>
@@ -2887,7 +2878,7 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
@@ -2902,7 +2893,7 @@
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
@@ -2917,7 +2908,7 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
@@ -2932,7 +2923,7 @@
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>2</v>
       </c>
@@ -2947,7 +2938,7 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
@@ -2962,7 +2953,7 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
@@ -2977,7 +2968,7 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
@@ -2992,7 +2983,7 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
@@ -3007,7 +2998,7 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
@@ -3022,7 +3013,7 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
@@ -3037,7 +3028,7 @@
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
@@ -3052,7 +3043,7 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
@@ -3067,7 +3058,7 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>2</v>
       </c>
@@ -3082,7 +3073,7 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>2</v>
       </c>
@@ -3097,7 +3088,7 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>2</v>
       </c>
@@ -3112,7 +3103,7 @@
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>2</v>
       </c>
@@ -3127,7 +3118,7 @@
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>2</v>
       </c>
@@ -3142,7 +3133,7 @@
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>3</v>
       </c>
@@ -3157,7 +3148,7 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>3</v>
       </c>
@@ -3174,7 +3165,7 @@
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>3</v>
       </c>
@@ -3189,7 +3180,7 @@
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>3</v>
       </c>
@@ -3204,7 +3195,7 @@
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>3</v>
       </c>
@@ -3219,7 +3210,7 @@
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>3</v>
       </c>
@@ -3234,7 +3225,7 @@
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>3</v>
       </c>
@@ -3251,7 +3242,7 @@
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>3</v>
       </c>
@@ -3266,7 +3257,7 @@
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>3</v>
       </c>
@@ -3283,7 +3274,7 @@
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>3</v>
       </c>
@@ -3300,7 +3291,7 @@
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>3</v>
       </c>
@@ -3315,7 +3306,7 @@
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>3</v>
       </c>
@@ -3330,7 +3321,7 @@
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>3</v>
       </c>
@@ -3345,7 +3336,7 @@
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>3</v>
       </c>
@@ -3360,7 +3351,7 @@
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>3</v>
       </c>
@@ -3375,7 +3366,7 @@
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>3</v>
       </c>
@@ -3390,7 +3381,7 @@
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>3</v>
       </c>
@@ -3405,7 +3396,7 @@
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>3</v>
       </c>
@@ -3417,12 +3408,12 @@
         <v>101</v>
       </c>
       <c r="E85" s="36" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>3</v>
       </c>
@@ -3439,7 +3430,7 @@
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>3</v>
       </c>
@@ -3454,7 +3445,7 @@
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>3</v>
       </c>
@@ -3469,7 +3460,7 @@
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>3</v>
       </c>
@@ -3488,7 +3479,7 @@
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>3</v>
       </c>
@@ -3507,7 +3498,7 @@
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>3</v>
       </c>
@@ -3524,7 +3515,7 @@
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>3</v>
       </c>
@@ -3541,7 +3532,7 @@
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>3</v>
       </c>
@@ -3558,7 +3549,7 @@
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>3</v>
       </c>
@@ -3573,7 +3564,7 @@
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>3</v>
       </c>
@@ -3588,7 +3579,7 @@
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>3</v>
       </c>
@@ -3603,7 +3594,7 @@
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="6">
         <f>COUNTA(B3:B96)</f>
@@ -3623,7 +3614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6" t="s">
@@ -3641,7 +3632,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G98"/>
+  <autoFilter ref="A2:G98" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="3">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:G1"/>
@@ -3654,23 +3645,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="1" max="1" width="9.109375" style="11"/>
     <col min="2" max="2" width="62" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.7109375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="62.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="11"/>
+    <col min="3" max="4" width="14.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="62.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="38" t="s">
         <v>114</v>
       </c>
@@ -3685,7 +3676,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="38"/>
       <c r="B2" s="38"/>
       <c r="C2" s="12" t="s">
@@ -3696,7 +3687,7 @@
       </c>
       <c r="E2" s="38"/>
     </row>
-    <row r="3" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>120</v>
       </c>
@@ -3707,7 +3698,7 @@
       <c r="D3" s="15"/>
       <c r="E3" s="16"/>
     </row>
-    <row r="4" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>122</v>
       </c>
@@ -3722,7 +3713,7 @@
       </c>
       <c r="E4" s="20"/>
     </row>
-    <row r="5" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>124</v>
       </c>
@@ -3737,7 +3728,7 @@
       </c>
       <c r="E5" s="22"/>
     </row>
-    <row r="6" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>126</v>
       </c>
@@ -3752,7 +3743,7 @@
       </c>
       <c r="E6" s="22"/>
     </row>
-    <row r="7" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>128</v>
       </c>
@@ -3767,7 +3758,7 @@
       </c>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>130</v>
       </c>
@@ -3782,7 +3773,7 @@
       </c>
       <c r="E8" s="23"/>
     </row>
-    <row r="9" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>132</v>
       </c>
@@ -3797,7 +3788,7 @@
       </c>
       <c r="E9" s="23"/>
     </row>
-    <row r="10" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>134</v>
       </c>
@@ -3812,7 +3803,7 @@
       </c>
       <c r="E10" s="23"/>
     </row>
-    <row r="11" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>136</v>
       </c>
@@ -3827,7 +3818,7 @@
       </c>
       <c r="E11" s="23"/>
     </row>
-    <row r="12" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>138</v>
       </c>
@@ -3842,7 +3833,7 @@
       </c>
       <c r="E12" s="23"/>
     </row>
-    <row r="13" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>140</v>
       </c>
@@ -3857,7 +3848,7 @@
       </c>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>142</v>
       </c>
@@ -3872,7 +3863,7 @@
       </c>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>144</v>
       </c>
@@ -3887,7 +3878,7 @@
       </c>
       <c r="E15" s="23"/>
     </row>
-    <row r="16" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>146</v>
       </c>
@@ -3902,7 +3893,7 @@
       </c>
       <c r="E16" s="23"/>
     </row>
-    <row r="17" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>148</v>
       </c>
@@ -3917,7 +3908,7 @@
       </c>
       <c r="E17" s="23"/>
     </row>
-    <row r="18" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>150</v>
       </c>
@@ -3932,7 +3923,7 @@
       </c>
       <c r="E18" s="23"/>
     </row>
-    <row r="19" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>152</v>
       </c>
@@ -3947,7 +3938,7 @@
       </c>
       <c r="E19" s="23"/>
     </row>
-    <row r="20" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>154</v>
       </c>
@@ -3962,7 +3953,7 @@
       </c>
       <c r="E20" s="23"/>
     </row>
-    <row r="21" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>259</v>
       </c>
@@ -3977,7 +3968,7 @@
       </c>
       <c r="E21" s="23"/>
     </row>
-    <row r="22" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>156</v>
       </c>
@@ -3992,7 +3983,7 @@
       </c>
       <c r="E22" s="23"/>
     </row>
-    <row r="23" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>158</v>
       </c>
@@ -4007,7 +3998,7 @@
       </c>
       <c r="E23" s="23"/>
     </row>
-    <row r="24" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="17" t="s">
         <v>160</v>
       </c>
@@ -4022,7 +4013,7 @@
       </c>
       <c r="E24" s="23"/>
     </row>
-    <row r="25" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>162</v>
       </c>
@@ -4037,7 +4028,7 @@
       </c>
       <c r="E25" s="23"/>
     </row>
-    <row r="26" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>164</v>
       </c>
@@ -4052,7 +4043,7 @@
       </c>
       <c r="E26" s="23"/>
     </row>
-    <row r="27" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>166</v>
       </c>
@@ -4065,7 +4056,7 @@
       </c>
       <c r="E27" s="23"/>
     </row>
-    <row r="28" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>168</v>
       </c>
@@ -4078,7 +4069,7 @@
       </c>
       <c r="E28" s="23"/>
     </row>
-    <row r="29" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>170</v>
       </c>
@@ -4093,7 +4084,7 @@
       </c>
       <c r="E29" s="23"/>
     </row>
-    <row r="30" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="17" t="s">
         <v>261</v>
       </c>
@@ -4108,7 +4099,7 @@
       </c>
       <c r="E30" s="23"/>
     </row>
-    <row r="31" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>173</v>
       </c>
@@ -4123,7 +4114,7 @@
       </c>
       <c r="E31" s="23"/>
     </row>
-    <row r="32" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="17" t="s">
         <v>175</v>
       </c>
@@ -4138,7 +4129,7 @@
       </c>
       <c r="E32" s="23"/>
     </row>
-    <row r="33" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>177</v>
       </c>
@@ -4153,7 +4144,7 @@
       </c>
       <c r="E33" s="23"/>
     </row>
-    <row r="34" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="17" t="s">
         <v>179</v>
       </c>
@@ -4168,7 +4159,7 @@
       </c>
       <c r="E34" s="23"/>
     </row>
-    <row r="35" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="17" t="s">
         <v>181</v>
       </c>
@@ -4183,7 +4174,7 @@
       </c>
       <c r="E35" s="23"/>
     </row>
-    <row r="36" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="17" t="s">
         <v>183</v>
       </c>
@@ -4196,7 +4187,7 @@
       <c r="D36" s="40"/>
       <c r="E36" s="23"/>
     </row>
-    <row r="37" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="17" t="s">
         <v>186</v>
       </c>
@@ -4211,7 +4202,7 @@
       </c>
       <c r="E37" s="23"/>
     </row>
-    <row r="38" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="17" t="s">
         <v>188</v>
       </c>
@@ -4226,7 +4217,7 @@
       </c>
       <c r="E38" s="23"/>
     </row>
-    <row r="39" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="17" t="s">
         <v>190</v>
       </c>
@@ -4241,7 +4232,7 @@
       </c>
       <c r="E39" s="23"/>
     </row>
-    <row r="40" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="17" t="s">
         <v>192</v>
       </c>
@@ -4256,7 +4247,7 @@
       </c>
       <c r="E40" s="23"/>
     </row>
-    <row r="41" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="17" t="s">
         <v>194</v>
       </c>
@@ -4271,7 +4262,7 @@
       </c>
       <c r="E41" s="23"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="17" t="s">
         <v>196</v>
       </c>
@@ -4286,7 +4277,7 @@
       </c>
       <c r="E42" s="23"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="17" t="s">
         <v>198</v>
       </c>
@@ -4301,7 +4292,7 @@
       </c>
       <c r="E43" s="23"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="17" t="s">
         <v>200</v>
       </c>
@@ -4316,7 +4307,7 @@
       </c>
       <c r="E44" s="23"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
         <v>257</v>
       </c>
@@ -4329,14 +4320,14 @@
       </c>
       <c r="E45" s="23"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="17"/>
       <c r="B46" s="18"/>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
       <c r="E46" s="23"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>202</v>
       </c>
@@ -4347,7 +4338,7 @@
       <c r="D47" s="15"/>
       <c r="E47" s="16"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="17" t="s">
         <v>204</v>
       </c>
@@ -4362,7 +4353,7 @@
       </c>
       <c r="E48" s="23"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="17" t="s">
         <v>206</v>
       </c>
@@ -4377,7 +4368,7 @@
       </c>
       <c r="E49" s="23"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="17" t="s">
         <v>208</v>
       </c>
@@ -4392,7 +4383,7 @@
       </c>
       <c r="E50" s="23"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
         <v>210</v>
       </c>
@@ -4407,7 +4398,7 @@
       </c>
       <c r="E51" s="23"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
         <v>212</v>
       </c>
@@ -4422,7 +4413,7 @@
       </c>
       <c r="E52" s="23"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="17" t="s">
         <v>214</v>
       </c>
@@ -4437,7 +4428,7 @@
       </c>
       <c r="E53" s="23"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="17" t="s">
         <v>216</v>
       </c>
@@ -4452,7 +4443,7 @@
       </c>
       <c r="E54" s="23"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
         <v>218</v>
       </c>
@@ -4467,7 +4458,7 @@
       </c>
       <c r="E55" s="23"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
         <v>220</v>
       </c>
@@ -4484,7 +4475,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="17" t="s">
         <v>223</v>
       </c>
@@ -4499,7 +4490,7 @@
       </c>
       <c r="E57" s="23"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="28" t="s">
         <v>225</v>
       </c>
@@ -4508,7 +4499,7 @@
       <c r="D58" s="27"/>
       <c r="E58" s="23"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="13" t="s">
         <v>226</v>
       </c>
@@ -4519,7 +4510,7 @@
       <c r="D59" s="15"/>
       <c r="E59" s="16"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="17" t="s">
         <v>228</v>
       </c>
@@ -4536,7 +4527,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="17" t="s">
         <v>231</v>
       </c>
@@ -4551,7 +4542,7 @@
       </c>
       <c r="E61" s="23"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
         <v>233</v>
       </c>
@@ -4566,7 +4557,7 @@
       </c>
       <c r="E62" s="23"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
         <v>235</v>
       </c>
@@ -4581,7 +4572,7 @@
       </c>
       <c r="E63" s="23"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>237</v>
       </c>
@@ -4596,7 +4587,7 @@
       </c>
       <c r="E64" s="23"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
         <v>239</v>
       </c>
@@ -4611,7 +4602,7 @@
       </c>
       <c r="E65" s="23"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>241</v>
       </c>
@@ -4628,7 +4619,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
         <v>244</v>
       </c>
@@ -4643,7 +4634,7 @@
       </c>
       <c r="E67" s="23"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
         <v>246</v>
       </c>
@@ -4656,7 +4647,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
         <v>249</v>
       </c>
@@ -4671,7 +4662,7 @@
       </c>
       <c r="E69" s="23"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="17" t="s">
         <v>251</v>
       </c>
@@ -4684,7 +4675,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="28" t="s">
         <v>254</v>
       </c>
@@ -4693,7 +4684,7 @@
       <c r="D71" s="30"/>
       <c r="E71" s="23"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="13" t="s">
         <v>255</v>
       </c>
@@ -4708,7 +4699,7 @@
       </c>
       <c r="E72" s="16"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="31"/>
       <c r="B73" s="32"/>
       <c r="C73" s="33">

</xml_diff>